<commit_message>
Finished Lab Print Sheet
</commit_message>
<xml_diff>
--- a/Charge 08 - T06.xlsx
+++ b/Charge 08 - T06.xlsx
@@ -9,206 +9,206 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Elements Data" sheetId="4" r:id="rId1"/>
-    <sheet name="Charge 08" sheetId="13" r:id="rId2"/>
-    <sheet name="A" sheetId="14" r:id="rId3"/>
-    <sheet name="B" sheetId="15" r:id="rId4"/>
-    <sheet name="C" sheetId="16" r:id="rId5"/>
-    <sheet name="D" sheetId="17" r:id="rId6"/>
-    <sheet name="E" sheetId="18" r:id="rId7"/>
-    <sheet name="Lab Print" sheetId="19" r:id="rId8"/>
+    <sheet name="Lab Print" sheetId="19" r:id="rId2"/>
+    <sheet name="Charge 08" sheetId="13" r:id="rId3"/>
+    <sheet name="A" sheetId="14" r:id="rId4"/>
+    <sheet name="B" sheetId="15" r:id="rId5"/>
+    <sheet name="C" sheetId="16" r:id="rId6"/>
+    <sheet name="D" sheetId="17" r:id="rId7"/>
+    <sheet name="E" sheetId="18" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">A!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">B!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'C'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Charge 08'!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">D!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">E!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">A!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">B!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'C'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Charge 08'!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">D!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">E!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Elements Data'!$A$1:$J$48</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">A!$B$2:$B$51</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">B!$B$2:$B$51</definedName>
-    <definedName name="solver_adj" localSheetId="4" hidden="1">'C'!$B$2:$B$51</definedName>
-    <definedName name="solver_adj" localSheetId="5" hidden="1">D!$B$2:$B$51</definedName>
-    <definedName name="solver_adj" localSheetId="6" hidden="1">E!$B$2:$B$51</definedName>
-    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">A!$B$2:$B$51</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">B!$B$2:$B$51</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'C'!$B$2:$B$51</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">D!$B$2:$B$51</definedName>
+    <definedName name="solver_adj" localSheetId="7" hidden="1">E!$B$2:$B$51</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
-    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_est" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">A!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">B!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'C'!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs1" localSheetId="5" hidden="1">D!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs1" localSheetId="6" hidden="1">E!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs2" localSheetId="2" hidden="1">A!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">B!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'C'!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs2" localSheetId="5" hidden="1">D!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs2" localSheetId="6" hidden="1">E!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs3" localSheetId="2" hidden="1">A!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">B!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs3" localSheetId="4" hidden="1">'C'!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs3" localSheetId="5" hidden="1">D!$B$2:$B$51</definedName>
-    <definedName name="solver_lhs3" localSheetId="6" hidden="1">E!$B$2:$B$51</definedName>
-    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">A!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">B!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'C'!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">D!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs1" localSheetId="7" hidden="1">E!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">A!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">B!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs2" localSheetId="5" hidden="1">'C'!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs2" localSheetId="6" hidden="1">D!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs2" localSheetId="7" hidden="1">E!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">A!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs3" localSheetId="4" hidden="1">B!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs3" localSheetId="5" hidden="1">'C'!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs3" localSheetId="6" hidden="1">D!$B$2:$B$51</definedName>
+    <definedName name="solver_lhs3" localSheetId="7" hidden="1">E!$B$2:$B$51</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mip" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_mni" localSheetId="7" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_mrt" localSheetId="7" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="6" hidden="1">2</definedName>
-    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_nod" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="6" hidden="1">3</definedName>
-    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">3</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">A!$F$4</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">B!$F$4</definedName>
-    <definedName name="solver_opt" localSheetId="4" hidden="1">'C'!$F$4</definedName>
-    <definedName name="solver_opt" localSheetId="5" hidden="1">D!$F$4</definedName>
-    <definedName name="solver_opt" localSheetId="6" hidden="1">E!$F$4</definedName>
-    <definedName name="solver_pre" localSheetId="2" hidden="1">0.001</definedName>
+    <definedName name="solver_nwt" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">A!$F$4</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">B!$F$4</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'C'!$F$4</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">D!$F$4</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">E!$F$4</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.001</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.001</definedName>
     <definedName name="solver_pre" localSheetId="5" hidden="1">0.001</definedName>
     <definedName name="solver_pre" localSheetId="6" hidden="1">0.001</definedName>
-    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_pre" localSheetId="7" hidden="1">0.001</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="2" hidden="1">4</definedName>
+    <definedName name="solver_rel1" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="3" hidden="1">4</definedName>
     <definedName name="solver_rel2" localSheetId="4" hidden="1">4</definedName>
     <definedName name="solver_rel2" localSheetId="5" hidden="1">4</definedName>
     <definedName name="solver_rel2" localSheetId="6" hidden="1">4</definedName>
-    <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="7" hidden="1">4</definedName>
     <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="6" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="7" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_rhs2" localSheetId="2" hidden="1">integer</definedName>
+    <definedName name="solver_rhs1" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_rhs2" localSheetId="3" hidden="1">integer</definedName>
     <definedName name="solver_rhs2" localSheetId="4" hidden="1">integer</definedName>
     <definedName name="solver_rhs2" localSheetId="5" hidden="1">integer</definedName>
     <definedName name="solver_rhs2" localSheetId="6" hidden="1">integer</definedName>
-    <definedName name="solver_rhs3" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="7" hidden="1">integer</definedName>
     <definedName name="solver_rhs3" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="6" hidden="1">0</definedName>
-    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rhs3" localSheetId="7" hidden="1">0</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="7" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_ssz" localSheetId="7" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_tim" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_tol" localSheetId="7" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_typ" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_typ" localSheetId="6" hidden="1">3</definedName>
-    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="174">
   <si>
     <t>Mg</t>
   </si>
@@ -743,6 +743,12 @@
   </si>
   <si>
     <t>Charge 08 - T06</t>
+  </si>
+  <si>
+    <t>Piece</t>
+  </si>
+  <si>
+    <t># Pieces</t>
   </si>
 </sst>
 </file>
@@ -753,7 +759,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -853,6 +859,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -946,7 +974,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1084,12 +1112,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1349,6 +1416,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1392,47 +1474,86 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4576,13 +4697,650 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="9.140625" style="55" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="55" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="55" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="55" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="182" t="str">
+        <f>'Charge 08'!A1:G1</f>
+        <v>Charge 08 - T06</v>
+      </c>
+      <c r="B1" s="183"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183"/>
+      <c r="E1" s="183"/>
+      <c r="F1" s="183"/>
+      <c r="G1" s="184"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="179" t="str">
+        <f>"Nominal  " &amp; 'Charge 08'!A3</f>
+        <v>Nominal  Mg65Zn30Ca5D0E0</v>
+      </c>
+      <c r="B2" s="180"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="181"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="179" t="str">
+        <f>"Actual  " &amp; 'Charge 08'!I3</f>
+        <v>Actual  Mg33.7Zn64.1Ca2.3D0E0</v>
+      </c>
+      <c r="B3" s="180"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="180"/>
+      <c r="F3" s="180"/>
+      <c r="G3" s="181"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="157" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="141" t="str">
+        <f>'Charge 08'!Q4</f>
+        <v>Mg</v>
+      </c>
+      <c r="C4" s="138" t="str">
+        <f>'Charge 08'!Q5</f>
+        <v>Zn</v>
+      </c>
+      <c r="D4" s="139" t="str">
+        <f>'Charge 08'!Q6</f>
+        <v>Ca</v>
+      </c>
+      <c r="E4" s="140" t="str">
+        <f>'Charge 08'!Q7</f>
+        <v>D</v>
+      </c>
+      <c r="F4" s="158" t="str">
+        <f>'Charge 08'!Q8</f>
+        <v>E</v>
+      </c>
+      <c r="G4" s="178" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="159"/>
+      <c r="B5" s="160" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="161" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="162" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="163" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="164" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="185" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
+        <v>1</v>
+      </c>
+      <c r="B6" s="109">
+        <f>'Charge 08'!B14</f>
+        <v>4.7270000000000003</v>
+      </c>
+      <c r="C6" s="165">
+        <f>'Charge 08'!E14</f>
+        <v>15.063000000000001</v>
+      </c>
+      <c r="D6" s="165">
+        <f>'Charge 08'!H14</f>
+        <v>6.08</v>
+      </c>
+      <c r="E6" s="165">
+        <f>'Charge 08'!K14</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="166">
+        <f>'Charge 08'!N14</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="186">
+        <f>COUNTIF(B6:B20, "&lt;&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="H6" s="137" t="str">
+        <f>B4</f>
+        <v>Mg</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="29">
+        <v>2</v>
+      </c>
+      <c r="B7" s="112">
+        <f>'Charge 08'!B15</f>
+        <v>4.8339999999999996</v>
+      </c>
+      <c r="C7" s="111">
+        <f>'Charge 08'!E15</f>
+        <v>16.469000000000001</v>
+      </c>
+      <c r="D7" s="111">
+        <f>'Charge 08'!H15</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="111">
+        <f>'Charge 08'!K15</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="110">
+        <f>'Charge 08'!N15</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="187">
+        <f>COUNTIF(C6:C20, "&lt;&gt;0")</f>
+        <v>6</v>
+      </c>
+      <c r="H7" s="188" t="str">
+        <f>C4</f>
+        <v>Zn</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
+        <v>3</v>
+      </c>
+      <c r="B8" s="112">
+        <f>'Charge 08'!B16</f>
+        <v>5.4930000000000003</v>
+      </c>
+      <c r="C8" s="111">
+        <f>'Charge 08'!E16</f>
+        <v>29.477</v>
+      </c>
+      <c r="D8" s="111">
+        <f>'Charge 08'!H16</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="111">
+        <f>'Charge 08'!K16</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="110">
+        <f>'Charge 08'!N16</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="187">
+        <f>COUNTIF(D6:D20, "&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="177" t="str">
+        <f>D4</f>
+        <v>Ca</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
+        <v>4</v>
+      </c>
+      <c r="B9" s="112">
+        <f>'Charge 08'!B17</f>
+        <v>7.2839999999999998</v>
+      </c>
+      <c r="C9" s="111">
+        <f>'Charge 08'!E17</f>
+        <v>12.114000000000001</v>
+      </c>
+      <c r="D9" s="111">
+        <f>'Charge 08'!H17</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="111">
+        <f>'Charge 08'!K17</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="110">
+        <f>'Charge 08'!N17</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="187">
+        <f>COUNTIF(E6:E20, "&lt;&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="189" t="str">
+        <f>E4</f>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="29">
+        <v>5</v>
+      </c>
+      <c r="B10" s="112">
+        <f>'Charge 08'!B18</f>
+        <v>7.6580000000000004</v>
+      </c>
+      <c r="C10" s="111">
+        <f>'Charge 08'!E18</f>
+        <v>12.664</v>
+      </c>
+      <c r="D10" s="111">
+        <f>'Charge 08'!H18</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="111">
+        <f>'Charge 08'!K18</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="110">
+        <f>'Charge 08'!N18</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="190">
+        <f>COUNTIF(F6:F20, "&lt;&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="191" t="str">
+        <f>F4</f>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <v>6</v>
+      </c>
+      <c r="B11" s="112">
+        <f>'Charge 08'!B19</f>
+        <v>8.6839999999999993</v>
+      </c>
+      <c r="C11" s="111">
+        <f>'Charge 08'!E19</f>
+        <v>193.78</v>
+      </c>
+      <c r="D11" s="111">
+        <f>'Charge 08'!H19</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="111">
+        <f>'Charge 08'!K19</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="110">
+        <f>'Charge 08'!N19</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="192">
+        <f>COUNTIF(B6:F20, "&lt;&gt;0")</f>
+        <v>15</v>
+      </c>
+      <c r="H11" s="193" t="str">
+        <f>G4</f>
+        <v>Alloy</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="29">
+        <v>7</v>
+      </c>
+      <c r="B12" s="112">
+        <f>'Charge 08'!B20</f>
+        <v>9.6129999999999995</v>
+      </c>
+      <c r="C12" s="111">
+        <f>'Charge 08'!E20</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="111">
+        <f>'Charge 08'!H20</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="111">
+        <f>'Charge 08'!K20</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="110">
+        <f>'Charge 08'!N20</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="110"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <v>8</v>
+      </c>
+      <c r="B13" s="112">
+        <f>'Charge 08'!B21</f>
+        <v>6.3310000000000004</v>
+      </c>
+      <c r="C13" s="111">
+        <f>'Charge 08'!E21</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="111">
+        <f>'Charge 08'!H21</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="111">
+        <f>'Charge 08'!K21</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="110">
+        <f>'Charge 08'!N21</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="110"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="29">
+        <v>9</v>
+      </c>
+      <c r="B14" s="112">
+        <f>'Charge 08'!B22</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="111">
+        <f>'Charge 08'!E22</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="111">
+        <f>'Charge 08'!H22</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="111">
+        <f>'Charge 08'!K22</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="110">
+        <f>'Charge 08'!N22</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="110"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="29">
+        <v>10</v>
+      </c>
+      <c r="B15" s="112">
+        <f>'Charge 08'!B23</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="111">
+        <f>'Charge 08'!E23</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="111">
+        <f>'Charge 08'!H23</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="111">
+        <f>'Charge 08'!K23</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="110">
+        <f>'Charge 08'!N23</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="110"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="29">
+        <v>11</v>
+      </c>
+      <c r="B16" s="112">
+        <f>'Charge 08'!B24</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="111">
+        <f>'Charge 08'!E24</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="111">
+        <f>'Charge 08'!H24</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="111">
+        <f>'Charge 08'!K24</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="110">
+        <f>'Charge 08'!N24</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="110"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
+        <v>12</v>
+      </c>
+      <c r="B17" s="112">
+        <f>'Charge 08'!B25</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="111">
+        <f>'Charge 08'!E25</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="111">
+        <f>'Charge 08'!H25</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="111">
+        <f>'Charge 08'!K25</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="110">
+        <f>'Charge 08'!N25</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="110"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
+        <v>13</v>
+      </c>
+      <c r="B18" s="112">
+        <f>'Charge 08'!B26</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="111">
+        <f>'Charge 08'!E26</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="111">
+        <f>'Charge 08'!H26</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="111">
+        <f>'Charge 08'!K26</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="110">
+        <f>'Charge 08'!N26</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="110"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>14</v>
+      </c>
+      <c r="B19" s="112">
+        <f>'Charge 08'!B27</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="111">
+        <f>'Charge 08'!E27</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="111">
+        <f>'Charge 08'!H27</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="111">
+        <f>'Charge 08'!K27</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="110">
+        <f>'Charge 08'!N27</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="110"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
+        <v>15</v>
+      </c>
+      <c r="B20" s="169">
+        <f>'Charge 08'!B28</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="118">
+        <f>'Charge 08'!E28</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="118">
+        <f>'Charge 08'!H28</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="118">
+        <f>'Charge 08'!K28</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="170">
+        <f>'Charge 08'!N28</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="110"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="171" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="74">
+        <f>SUM(B6:B20)</f>
+        <v>54.624000000000002</v>
+      </c>
+      <c r="C21" s="38">
+        <f>SUM(C6:C20)</f>
+        <v>279.56700000000001</v>
+      </c>
+      <c r="D21" s="172">
+        <f>SUM(D6:D20)</f>
+        <v>6.08</v>
+      </c>
+      <c r="E21" s="38">
+        <f>SUM(E6:E20)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="173">
+        <f>SUM(F6:F20)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="173">
+        <f>SUM(B21:F21)</f>
+        <v>340.27100000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="113" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="174">
+        <f>'Charge 08'!F4</f>
+        <v>47.921999999999997</v>
+      </c>
+      <c r="C22" s="156">
+        <f>'Charge 08'!F5</f>
+        <v>59.499000000000002</v>
+      </c>
+      <c r="D22" s="156">
+        <f>'Charge 08'!F6</f>
+        <v>6.0789999999999997</v>
+      </c>
+      <c r="E22" s="156">
+        <f>'Charge 08'!F7</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="167">
+        <f>'Charge 08'!F8</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="72">
+        <f>SUM(B22:F22)</f>
+        <v>113.49999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="176" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="175">
+        <f>B21-B22</f>
+        <v>6.7020000000000053</v>
+      </c>
+      <c r="C23" s="168">
+        <f t="shared" ref="C23:G23" si="0">C21-C22</f>
+        <v>220.06800000000001</v>
+      </c>
+      <c r="D23" s="168">
+        <f t="shared" si="0"/>
+        <v>1.000000000000334E-3</v>
+      </c>
+      <c r="E23" s="168">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="117">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="117">
+        <f t="shared" si="0"/>
+        <v>226.77100000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:AB93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4604,15 +5362,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="142" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="56" t="s">
@@ -4652,7 +5410,7 @@
       </c>
       <c r="I3" s="64" t="str">
         <f>Q4 &amp; ROUND(N4,3)*100 &amp; Q5 &amp; ROUND(N5,3)*100 &amp; Q6 &amp; ROUND(N6,3)*100 &amp; Q7 &amp; ROUND(N7,3)*100 &amp; Q8 &amp; ROUND(N8,3)*100</f>
-        <v>Mg67.4Zn28Ca4.6D0E0</v>
+        <v>Mg33.7Zn64.1Ca2.3D0E0</v>
       </c>
       <c r="J3" s="65"/>
       <c r="K3" s="66" t="s">
@@ -4737,19 +5495,19 @@
       <c r="J4" s="28"/>
       <c r="K4" s="74">
         <f>B29</f>
-        <v>54.623999999999995</v>
+        <v>54.624000000000002</v>
       </c>
       <c r="L4" s="75">
         <f>K4/$K$9</f>
-        <v>0.44879347317049123</v>
+        <v>0.1605308709822465</v>
       </c>
       <c r="M4" s="25">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>1.8465067811993058E-2</v>
+        <v>6.604849659833224E-3</v>
       </c>
       <c r="N4" s="120">
         <f>M4/$M$9</f>
-        <v>0.67444898947468235</v>
+        <v>0.33669270145147684</v>
       </c>
       <c r="P4" s="17">
         <v>1</v>
@@ -4830,19 +5588,19 @@
       <c r="J5" s="29"/>
       <c r="K5" s="77">
         <f>E29</f>
-        <v>61.009</v>
+        <v>279.56700000000001</v>
       </c>
       <c r="L5" s="78">
         <f>K5/$K$9</f>
-        <v>0.50125294750766147</v>
+        <v>0.82160101801211383</v>
       </c>
       <c r="M5" s="26">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>7.6665282112456249E-3</v>
+        <v>1.2566165275031564E-2</v>
       </c>
       <c r="N5" s="121">
         <f>M5/$M$9</f>
-        <v>0.28002508615188504</v>
+        <v>0.64058023289555865</v>
       </c>
       <c r="P5" s="17">
         <v>2</v>
@@ -4927,15 +5685,15 @@
       </c>
       <c r="L6" s="78">
         <f>K6/$K$9</f>
-        <v>4.9953579321847297E-2</v>
+        <v>1.7868111005639623E-2</v>
       </c>
       <c r="M6" s="26">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>1.2464089855244098E-3</v>
+        <v>4.4583340001096914E-4</v>
       </c>
       <c r="N6" s="121">
         <f>M6/$M$9</f>
-        <v>4.5525924373432683E-2</v>
+        <v>2.2727065652964524E-2</v>
       </c>
       <c r="P6" s="17">
         <v>3</v>
@@ -5199,7 +5957,7 @@
       </c>
       <c r="K9" s="122">
         <f>SUM(K4:K8)</f>
-        <v>121.71299999999999</v>
+        <v>340.27100000000002</v>
       </c>
       <c r="L9" s="86">
         <f>SUM(L4:L8)</f>
@@ -5207,7 +5965,7 @@
       </c>
       <c r="M9" s="123">
         <f>SUM(M4:M8)</f>
-        <v>2.7378005008763091E-2</v>
+        <v>1.9616848334875758E-2</v>
       </c>
       <c r="N9" s="87">
         <f>SUM(N4:N8)</f>
@@ -5247,35 +6005,35 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="141" t="str">
+      <c r="A12" s="146" t="str">
         <f>$Q$4</f>
         <v>Mg</v>
       </c>
-      <c r="B12" s="142"/>
+      <c r="B12" s="147"/>
       <c r="C12" s="91"/>
-      <c r="D12" s="143" t="str">
+      <c r="D12" s="148" t="str">
         <f>$Q$5</f>
         <v>Zn</v>
       </c>
-      <c r="E12" s="144"/>
+      <c r="E12" s="149"/>
       <c r="F12" s="91"/>
-      <c r="G12" s="145" t="str">
+      <c r="G12" s="150" t="str">
         <f>$Q$6</f>
         <v>Ca</v>
       </c>
-      <c r="H12" s="146"/>
+      <c r="H12" s="151"/>
       <c r="I12" s="92"/>
-      <c r="J12" s="147" t="str">
+      <c r="J12" s="152" t="str">
         <f>$Q$7</f>
         <v>D</v>
       </c>
-      <c r="K12" s="148"/>
+      <c r="K12" s="153"/>
       <c r="L12" s="91"/>
-      <c r="M12" s="149" t="str">
+      <c r="M12" s="154" t="str">
         <f>$Q$8</f>
         <v>E</v>
       </c>
-      <c r="N12" s="150"/>
+      <c r="N12" s="155"/>
       <c r="P12" s="93" t="s">
         <v>90</v>
       </c>
@@ -5384,6 +6142,8 @@
       <c r="R14" s="11"/>
       <c r="S14" s="8"/>
       <c r="T14" s="9"/>
+      <c r="V14"/>
+      <c r="W14"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="132">
@@ -5434,6 +6194,8 @@
       <c r="R15" s="11"/>
       <c r="S15" s="8"/>
       <c r="T15" s="9"/>
+      <c r="V15"/>
+      <c r="W15"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="132">
@@ -5484,6 +6246,8 @@
       <c r="R16" s="11"/>
       <c r="S16" s="8"/>
       <c r="T16" s="9"/>
+      <c r="V16"/>
+      <c r="W16"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="132">
@@ -5491,7 +6255,7 @@
       </c>
       <c r="B17" s="110">
         <f>A!C5</f>
-        <v>6.3310000000000004</v>
+        <v>7.2839999999999998</v>
       </c>
       <c r="C17" s="111"/>
       <c r="D17" s="132">
@@ -5499,7 +6263,7 @@
       </c>
       <c r="E17" s="110">
         <f>B!C5</f>
-        <v>0</v>
+        <v>12.114000000000001</v>
       </c>
       <c r="F17" s="111"/>
       <c r="G17" s="132">
@@ -5534,6 +6298,8 @@
       <c r="R17" s="11"/>
       <c r="S17" s="8"/>
       <c r="T17" s="9"/>
+      <c r="V17"/>
+      <c r="W17"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="132">
@@ -5541,7 +6307,7 @@
       </c>
       <c r="B18" s="110">
         <f>A!C6</f>
-        <v>7.2839999999999998</v>
+        <v>7.6580000000000004</v>
       </c>
       <c r="C18" s="111"/>
       <c r="D18" s="132">
@@ -5549,7 +6315,7 @@
       </c>
       <c r="E18" s="110">
         <f>B!C6</f>
-        <v>0</v>
+        <v>12.664</v>
       </c>
       <c r="F18" s="111"/>
       <c r="G18" s="132">
@@ -5586,6 +6352,8 @@
       </c>
       <c r="S18" s="8"/>
       <c r="T18" s="9"/>
+      <c r="V18"/>
+      <c r="W18"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="132">
@@ -5593,7 +6361,7 @@
       </c>
       <c r="B19" s="110">
         <f>A!C7</f>
-        <v>7.6580000000000004</v>
+        <v>8.6839999999999993</v>
       </c>
       <c r="C19" s="111"/>
       <c r="D19" s="132">
@@ -5601,7 +6369,7 @@
       </c>
       <c r="E19" s="110">
         <f>B!C7</f>
-        <v>0</v>
+        <v>193.78</v>
       </c>
       <c r="F19" s="111"/>
       <c r="G19" s="132">
@@ -5634,6 +6402,8 @@
       <c r="R19" s="11"/>
       <c r="S19" s="8"/>
       <c r="T19" s="9"/>
+      <c r="V19"/>
+      <c r="W19"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="132">
@@ -5641,7 +6411,7 @@
       </c>
       <c r="B20" s="110">
         <f>A!C8</f>
-        <v>8.6839999999999993</v>
+        <v>9.6129999999999995</v>
       </c>
       <c r="C20" s="111"/>
       <c r="D20" s="132">
@@ -5682,6 +6452,8 @@
       <c r="R20" s="11"/>
       <c r="S20" s="8"/>
       <c r="T20" s="9"/>
+      <c r="V20"/>
+      <c r="W20"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="132">
@@ -5689,7 +6461,7 @@
       </c>
       <c r="B21" s="110">
         <f>A!C9</f>
-        <v>9.6129999999999995</v>
+        <v>6.3310000000000004</v>
       </c>
       <c r="C21" s="111"/>
       <c r="D21" s="132">
@@ -5730,6 +6502,8 @@
       <c r="R21" s="11"/>
       <c r="S21" s="8"/>
       <c r="T21" s="9"/>
+      <c r="V21"/>
+      <c r="W21"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="132">
@@ -6031,7 +6805,7 @@
       </c>
       <c r="B29" s="114">
         <f>SUM(B14:B28)</f>
-        <v>54.623999999999995</v>
+        <v>54.624000000000002</v>
       </c>
       <c r="C29" s="111"/>
       <c r="D29" s="113" t="s">
@@ -6039,7 +6813,7 @@
       </c>
       <c r="E29" s="115">
         <f>SUM(E14:E28)</f>
-        <v>61.009</v>
+        <v>279.56700000000001</v>
       </c>
       <c r="F29" s="111"/>
       <c r="G29" s="113" t="s">
@@ -6072,7 +6846,7 @@
       </c>
       <c r="B30" s="117">
         <f>B29-$F$4</f>
-        <v>6.7019999999999982</v>
+        <v>6.7020000000000053</v>
       </c>
       <c r="C30" s="118"/>
       <c r="D30" s="116" t="s">
@@ -6080,7 +6854,7 @@
       </c>
       <c r="E30" s="117">
         <f>E29-$F$5</f>
-        <v>1.509999999999998</v>
+        <v>220.06800000000001</v>
       </c>
       <c r="F30" s="118"/>
       <c r="G30" s="116" t="s">
@@ -6109,35 +6883,35 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:27" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="138" t="s">
+      <c r="A32" s="143" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="139"/>
-      <c r="C32" s="139"/>
-      <c r="D32" s="139"/>
-      <c r="E32" s="139"/>
-      <c r="F32" s="139"/>
-      <c r="G32" s="139"/>
-      <c r="H32" s="139"/>
-      <c r="I32" s="139"/>
-      <c r="J32" s="139"/>
-      <c r="K32" s="139"/>
-      <c r="L32" s="139"/>
-      <c r="M32" s="139"/>
-      <c r="N32" s="139"/>
-      <c r="O32" s="139"/>
-      <c r="P32" s="139"/>
-      <c r="Q32" s="139"/>
-      <c r="R32" s="139"/>
-      <c r="S32" s="139"/>
-      <c r="T32" s="139"/>
-      <c r="U32" s="139"/>
-      <c r="V32" s="139"/>
-      <c r="W32" s="139"/>
-      <c r="X32" s="139"/>
-      <c r="Y32" s="139"/>
-      <c r="Z32" s="139"/>
-      <c r="AA32" s="140"/>
+      <c r="B32" s="144"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="144"/>
+      <c r="H32" s="144"/>
+      <c r="I32" s="144"/>
+      <c r="J32" s="144"/>
+      <c r="K32" s="144"/>
+      <c r="L32" s="144"/>
+      <c r="M32" s="144"/>
+      <c r="N32" s="144"/>
+      <c r="O32" s="144"/>
+      <c r="P32" s="144"/>
+      <c r="Q32" s="144"/>
+      <c r="R32" s="144"/>
+      <c r="S32" s="144"/>
+      <c r="T32" s="144"/>
+      <c r="U32" s="144"/>
+      <c r="V32" s="144"/>
+      <c r="W32" s="144"/>
+      <c r="X32" s="144"/>
+      <c r="Y32" s="144"/>
+      <c r="Z32" s="144"/>
+      <c r="AA32" s="145"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
@@ -7392,7 +8166,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFDF4158"/>
@@ -7401,7 +8175,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -7442,12 +8216,12 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
+        <f>IF(A2=0, 0, A2*B2)</f>
         <v>4.7270000000000003</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>54.623999999999995</v>
+        <v>54.624000000000002</v>
       </c>
       <c r="E2" s="133" t="s">
         <v>109</v>
@@ -7465,7 +8239,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f>IF(A3=0, 0, A3*B3)</f>
         <v>4.8339999999999996</v>
       </c>
       <c r="D3" s="1"/>
@@ -7474,7 +8248,7 @@
       </c>
       <c r="F3" s="135">
         <f>SUM(C:C)</f>
-        <v>54.623999999999995</v>
+        <v>54.624000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7485,7 +8259,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f>IF(A4=0, 0, A4*B4)</f>
         <v>5.4930000000000003</v>
       </c>
       <c r="D4" s="1"/>
@@ -7494,67 +8268,67 @@
       </c>
       <c r="F4" s="135">
         <f>F3-F2</f>
-        <v>6.7019999999999982</v>
+        <v>6.7020000000000053</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="131">
-        <v>6.3310000000000004</v>
+      <c r="A5" s="130">
+        <v>7.2839999999999998</v>
       </c>
       <c r="B5" s="130">
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>6.3310000000000004</v>
+        <f>IF(A5=0, 0, A5*B5)</f>
+        <v>7.2839999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="130">
-        <v>7.2839999999999998</v>
+        <v>7.6580000000000004</v>
       </c>
       <c r="B6" s="130">
         <v>1</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>7.2839999999999998</v>
+        <f>IF(A6=0, 0, A6*B6)</f>
+        <v>7.6580000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="130">
-        <v>7.6580000000000004</v>
+        <v>8.6839999999999993</v>
       </c>
       <c r="B7" s="130">
         <v>1</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>7.6580000000000004</v>
+        <f>IF(A7=0, 0, A7*B7)</f>
+        <v>8.6839999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="130">
-        <v>8.6839999999999993</v>
+      <c r="A8" s="131">
+        <v>9.6129999999999995</v>
       </c>
       <c r="B8" s="130">
         <v>1</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>8.6839999999999993</v>
+        <f>IF(A8=0, 0, A8*B8)</f>
+        <v>9.6129999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="131">
-        <v>9.6129999999999995</v>
+        <v>6.3310000000000004</v>
       </c>
       <c r="B9" s="130">
         <v>1</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>9.6129999999999995</v>
+        <f>IF(A9=0, 0, A9*B9)</f>
+        <v>6.3310000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -7563,7 +8337,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
@@ -7573,7 +8347,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
@@ -7583,7 +8357,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
@@ -7593,7 +8367,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
@@ -7603,7 +8377,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
@@ -7613,7 +8387,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
@@ -7623,7 +8397,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
@@ -7633,7 +8407,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
@@ -7643,7 +8417,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
@@ -7653,7 +8427,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
@@ -7663,7 +8437,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
@@ -7673,7 +8447,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
@@ -7683,7 +8457,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
@@ -7693,7 +8467,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
@@ -7703,7 +8477,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
@@ -7713,7 +8487,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
@@ -7723,7 +8497,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
@@ -7733,7 +8507,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -7743,7 +8517,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -7753,7 +8527,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -7763,7 +8537,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -7773,7 +8547,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -7783,7 +8557,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -7793,7 +8567,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -7803,7 +8577,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -7813,7 +8587,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -7823,7 +8597,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -7833,7 +8607,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -7843,7 +8617,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -7853,7 +8627,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -7863,7 +8637,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -7873,7 +8647,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -7883,7 +8657,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -7893,7 +8667,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -7903,7 +8677,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -7913,7 +8687,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -7923,7 +8697,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -7933,7 +8707,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -7943,7 +8717,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -7953,7 +8727,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -7963,7 +8737,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -7973,7 +8747,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
@@ -7988,7 +8762,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -7997,7 +8771,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -8043,7 +8817,7 @@
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>61.009</v>
+        <v>279.56700000000001</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>109</v>
@@ -8069,7 +8843,7 @@
       </c>
       <c r="F3" s="53">
         <f>SUM(C:C)</f>
-        <v>61.009</v>
+        <v>279.56700000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -8088,7 +8862,7 @@
       </c>
       <c r="F4" s="53">
         <f>F3-F2</f>
-        <v>1.509999999999998</v>
+        <v>220.06800000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8096,11 +8870,11 @@
         <v>12.114000000000001</v>
       </c>
       <c r="B5" s="130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.114000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8108,11 +8882,11 @@
         <v>12.664</v>
       </c>
       <c r="B6" s="130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.664</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8120,11 +8894,11 @@
         <v>193.78</v>
       </c>
       <c r="B7" s="130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>193.78</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8578,7 +9352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -8587,7 +9361,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9158,7 +9932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
@@ -9167,7 +9941,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A28"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9736,7 +10510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -9745,7 +10519,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A28"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -10312,512 +11086,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF002060"/>
-  </sheetPr>
-  <dimension ref="A1:G20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="55"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="166" t="str">
-        <f>'Charge 08'!A1:G1</f>
-        <v>Charge 08 - T06</v>
-      </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="151" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="160" t="str">
-        <f>'Charge 08'!Q4</f>
-        <v>Mg</v>
-      </c>
-      <c r="C2" s="152" t="str">
-        <f>'Charge 08'!Q5</f>
-        <v>Zn</v>
-      </c>
-      <c r="D2" s="153" t="str">
-        <f>'Charge 08'!Q6</f>
-        <v>Ca</v>
-      </c>
-      <c r="E2" s="154" t="str">
-        <f>'Charge 08'!Q7</f>
-        <v>D</v>
-      </c>
-      <c r="F2" s="155" t="str">
-        <f>'Charge 08'!Q8</f>
-        <v>E</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="151"/>
-      <c r="B3" s="161" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="162" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="163" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="164" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="165" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="156">
-        <v>1</v>
-      </c>
-      <c r="B4" s="111">
-        <f>'Charge 08'!B14</f>
-        <v>4.7270000000000003</v>
-      </c>
-      <c r="C4" s="111">
-        <f>'Charge 08'!E14</f>
-        <v>15.063000000000001</v>
-      </c>
-      <c r="D4" s="111">
-        <f>'Charge 08'!H14</f>
-        <v>6.08</v>
-      </c>
-      <c r="E4" s="111">
-        <f>'Charge 08'!K14</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="111">
-        <f>'Charge 08'!N14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="156">
-        <v>2</v>
-      </c>
-      <c r="B5" s="111">
-        <f>'Charge 08'!B15</f>
-        <v>4.8339999999999996</v>
-      </c>
-      <c r="C5" s="111">
-        <f>'Charge 08'!E15</f>
-        <v>16.469000000000001</v>
-      </c>
-      <c r="D5" s="111">
-        <f>'Charge 08'!H15</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="111">
-        <f>'Charge 08'!K15</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="111">
-        <f>'Charge 08'!N15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="156">
-        <v>3</v>
-      </c>
-      <c r="B6" s="111">
-        <f>'Charge 08'!B16</f>
-        <v>5.4930000000000003</v>
-      </c>
-      <c r="C6" s="111">
-        <f>'Charge 08'!E16</f>
-        <v>29.477</v>
-      </c>
-      <c r="D6" s="111">
-        <f>'Charge 08'!H16</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="111">
-        <f>'Charge 08'!K16</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="111">
-        <f>'Charge 08'!N16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="156">
-        <v>4</v>
-      </c>
-      <c r="B7" s="111">
-        <f>'Charge 08'!B17</f>
-        <v>6.3310000000000004</v>
-      </c>
-      <c r="C7" s="111">
-        <f>'Charge 08'!E17</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="111">
-        <f>'Charge 08'!H17</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="111">
-        <f>'Charge 08'!K17</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="111">
-        <f>'Charge 08'!N17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="156">
-        <v>5</v>
-      </c>
-      <c r="B8" s="111">
-        <f>'Charge 08'!B18</f>
-        <v>7.2839999999999998</v>
-      </c>
-      <c r="C8" s="111">
-        <f>'Charge 08'!E18</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="111">
-        <f>'Charge 08'!H18</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="111">
-        <f>'Charge 08'!K18</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="111">
-        <f>'Charge 08'!N18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="156">
-        <v>6</v>
-      </c>
-      <c r="B9" s="111">
-        <f>'Charge 08'!B19</f>
-        <v>7.6580000000000004</v>
-      </c>
-      <c r="C9" s="111">
-        <f>'Charge 08'!E19</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="111">
-        <f>'Charge 08'!H19</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="111">
-        <f>'Charge 08'!K19</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="111">
-        <f>'Charge 08'!N19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="156">
-        <v>7</v>
-      </c>
-      <c r="B10" s="111">
-        <f>'Charge 08'!B20</f>
-        <v>8.6839999999999993</v>
-      </c>
-      <c r="C10" s="111">
-        <f>'Charge 08'!E20</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="111">
-        <f>'Charge 08'!H20</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="111">
-        <f>'Charge 08'!K20</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="111">
-        <f>'Charge 08'!N20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="156">
-        <v>8</v>
-      </c>
-      <c r="B11" s="111">
-        <f>'Charge 08'!B21</f>
-        <v>9.6129999999999995</v>
-      </c>
-      <c r="C11" s="111">
-        <f>'Charge 08'!E21</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="111">
-        <f>'Charge 08'!H21</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="111">
-        <f>'Charge 08'!K21</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="111">
-        <f>'Charge 08'!N21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="156">
-        <v>9</v>
-      </c>
-      <c r="B12" s="111">
-        <f>'Charge 08'!B22</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="111">
-        <f>'Charge 08'!E22</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="111">
-        <f>'Charge 08'!H22</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="111">
-        <f>'Charge 08'!K22</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="111">
-        <f>'Charge 08'!N22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="156">
-        <v>10</v>
-      </c>
-      <c r="B13" s="111">
-        <f>'Charge 08'!B23</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="111">
-        <f>'Charge 08'!E23</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="111">
-        <f>'Charge 08'!H23</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="111">
-        <f>'Charge 08'!K23</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="111">
-        <f>'Charge 08'!N23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="156">
-        <v>11</v>
-      </c>
-      <c r="B14" s="111">
-        <f>'Charge 08'!B24</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="111">
-        <f>'Charge 08'!E24</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="111">
-        <f>'Charge 08'!H24</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="111">
-        <f>'Charge 08'!K24</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="111">
-        <f>'Charge 08'!N24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="156">
-        <v>12</v>
-      </c>
-      <c r="B15" s="111">
-        <f>'Charge 08'!B25</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="111">
-        <f>'Charge 08'!E25</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="111">
-        <f>'Charge 08'!H25</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="111">
-        <f>'Charge 08'!K25</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="111">
-        <f>'Charge 08'!N25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="156">
-        <v>13</v>
-      </c>
-      <c r="B16" s="111">
-        <f>'Charge 08'!B26</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="111">
-        <f>'Charge 08'!E26</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="111">
-        <f>'Charge 08'!H26</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="111">
-        <f>'Charge 08'!K26</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="111">
-        <f>'Charge 08'!N26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="156">
-        <v>14</v>
-      </c>
-      <c r="B17" s="111">
-        <f>'Charge 08'!B27</f>
-        <v>0</v>
-      </c>
-      <c r="C17" s="111">
-        <f>'Charge 08'!E27</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="111">
-        <f>'Charge 08'!H27</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="111">
-        <f>'Charge 08'!K27</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="111">
-        <f>'Charge 08'!N27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="156">
-        <v>15</v>
-      </c>
-      <c r="B18" s="111">
-        <f>'Charge 08'!B28</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="111">
-        <f>'Charge 08'!E28</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="111">
-        <f>'Charge 08'!H28</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="111">
-        <f>'Charge 08'!K28</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="111">
-        <f>'Charge 08'!N28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="157" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="71">
-        <f>SUM(B4:B18)</f>
-        <v>54.623999999999995</v>
-      </c>
-      <c r="C19" s="39">
-        <f>SUM(C4:C18)</f>
-        <v>61.009</v>
-      </c>
-      <c r="D19" s="71">
-        <f>SUM(D4:D18)</f>
-        <v>6.08</v>
-      </c>
-      <c r="E19" s="39">
-        <f>SUM(E4:E18)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="71">
-        <f>SUM(F4:F18)</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="167">
-        <f>SUM(B19:F19)</f>
-        <v>121.71299999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="158" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="159">
-        <f>B19-'Charge 08'!F4</f>
-        <v>6.7019999999999982</v>
-      </c>
-      <c r="C20" s="159">
-        <f>C19-'Charge 08'!F5</f>
-        <v>1.509999999999998</v>
-      </c>
-      <c r="D20" s="159">
-        <f>D19-'Charge 08'!F6</f>
-        <v>1.000000000000334E-3</v>
-      </c>
-      <c r="E20" s="159">
-        <f>E19-'Charge 08'!F7</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="159">
-        <f>F19-'Charge 08'!F8</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Alloy name now only includes elements over 0.0at% or 0.0wt%
</commit_message>
<xml_diff>
--- a/Charge 08 - T06.xlsx
+++ b/Charge 08 - T06.xlsx
@@ -1425,11 +1425,79 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1474,84 +1542,16 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4685,6 +4685,7 @@
     <row r="118" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="119" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A1:J48">
     <sortState ref="A2:I101">
       <sortCondition ref="B1:B48"/>
@@ -4715,46 +4716,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="182" t="str">
+      <c r="A1" s="170" t="str">
         <f>'Charge 08'!A1:G1</f>
         <v>Charge 08 - T06</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
-      <c r="G1" s="184"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="172"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="179" t="str">
+      <c r="A2" s="173" t="str">
         <f>"Nominal  " &amp; 'Charge 08'!A3</f>
-        <v>Nominal  Mg65Zn30Ca5D0E0</v>
-      </c>
-      <c r="B2" s="180"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="180"/>
-      <c r="F2" s="180"/>
-      <c r="G2" s="181"/>
+        <v>Nominal  Mg65Zn30Ca5</v>
+      </c>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="179" t="str">
+      <c r="A3" s="173" t="str">
         <f>"Actual  " &amp; 'Charge 08'!I3</f>
-        <v>Actual  Mg33.7Zn64.1Ca2.3D0E0</v>
-      </c>
-      <c r="B3" s="180"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="180"/>
-      <c r="G3" s="181"/>
+        <v>Actual  Mg33.7Zn64.1Ca2.3</v>
+      </c>
+      <c r="B3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="175"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="157" t="s">
+      <c r="A4" s="168" t="s">
         <v>172</v>
       </c>
-      <c r="B4" s="141" t="str">
+      <c r="B4" s="140" t="str">
         <f>'Charge 08'!Q4</f>
         <v>Mg</v>
       </c>
@@ -4766,36 +4767,36 @@
         <f>'Charge 08'!Q6</f>
         <v>Ca</v>
       </c>
-      <c r="E4" s="140" t="str">
+      <c r="E4" s="190" t="str">
         <f>'Charge 08'!Q7</f>
         <v>D</v>
       </c>
-      <c r="F4" s="158" t="str">
+      <c r="F4" s="164" t="str">
         <f>'Charge 08'!Q8</f>
         <v>E</v>
       </c>
-      <c r="G4" s="178" t="s">
+      <c r="G4" s="159" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="159"/>
-      <c r="B5" s="160" t="s">
+      <c r="A5" s="169"/>
+      <c r="B5" s="143" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="161" t="s">
+      <c r="C5" s="144" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="162" t="s">
+      <c r="D5" s="145" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="163" t="s">
+      <c r="E5" s="191" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="164" t="s">
+      <c r="F5" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="185" t="s">
+      <c r="G5" s="160" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4807,23 +4808,23 @@
         <f>'Charge 08'!B14</f>
         <v>4.7270000000000003</v>
       </c>
-      <c r="C6" s="165">
+      <c r="C6" s="146">
         <f>'Charge 08'!E14</f>
         <v>15.063000000000001</v>
       </c>
-      <c r="D6" s="165">
+      <c r="D6" s="146">
         <f>'Charge 08'!H14</f>
         <v>6.08</v>
       </c>
-      <c r="E6" s="165">
+      <c r="E6" s="146">
         <f>'Charge 08'!K14</f>
         <v>0</v>
       </c>
-      <c r="F6" s="166">
+      <c r="F6" s="147">
         <f>'Charge 08'!N14</f>
         <v>0</v>
       </c>
-      <c r="G6" s="186">
+      <c r="G6" s="161">
         <f>COUNTIF(B6:B20, "&lt;&gt;0")</f>
         <v>8</v>
       </c>
@@ -4856,11 +4857,11 @@
         <f>'Charge 08'!N15</f>
         <v>0</v>
       </c>
-      <c r="G7" s="187">
+      <c r="G7" s="162">
         <f>COUNTIF(C6:C20, "&lt;&gt;0")</f>
         <v>6</v>
       </c>
-      <c r="H7" s="188" t="str">
+      <c r="H7" s="163" t="str">
         <f>C4</f>
         <v>Zn</v>
       </c>
@@ -4889,11 +4890,11 @@
         <f>'Charge 08'!N16</f>
         <v>0</v>
       </c>
-      <c r="G8" s="187">
+      <c r="G8" s="162">
         <f>COUNTIF(D6:D20, "&lt;&gt;0")</f>
         <v>1</v>
       </c>
-      <c r="H8" s="177" t="str">
+      <c r="H8" s="158" t="str">
         <f>D4</f>
         <v>Ca</v>
       </c>
@@ -4922,11 +4923,11 @@
         <f>'Charge 08'!N17</f>
         <v>0</v>
       </c>
-      <c r="G9" s="187">
+      <c r="G9" s="162">
         <f>COUNTIF(E6:E20, "&lt;&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="H9" s="189" t="str">
+      <c r="H9" s="142" t="str">
         <f>E4</f>
         <v>D</v>
       </c>
@@ -4955,11 +4956,11 @@
         <f>'Charge 08'!N18</f>
         <v>0</v>
       </c>
-      <c r="G10" s="190">
+      <c r="G10" s="165">
         <f>COUNTIF(F6:F20, "&lt;&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="H10" s="191" t="str">
+      <c r="H10" s="193" t="str">
         <f>F4</f>
         <v>E</v>
       </c>
@@ -4988,11 +4989,11 @@
         <f>'Charge 08'!N19</f>
         <v>0</v>
       </c>
-      <c r="G11" s="192">
+      <c r="G11" s="166">
         <f>COUNTIF(B6:F20, "&lt;&gt;0")</f>
         <v>15</v>
       </c>
-      <c r="H11" s="193" t="str">
+      <c r="H11" s="167" t="str">
         <f>G4</f>
         <v>Alloy</v>
       </c>
@@ -5209,7 +5210,7 @@
       <c r="A20" s="29">
         <v>15</v>
       </c>
-      <c r="B20" s="169">
+      <c r="B20" s="150">
         <f>'Charge 08'!B28</f>
         <v>0</v>
       </c>
@@ -5225,14 +5226,14 @@
         <f>'Charge 08'!K28</f>
         <v>0</v>
       </c>
-      <c r="F20" s="170">
+      <c r="F20" s="151">
         <f>'Charge 08'!N28</f>
         <v>0</v>
       </c>
       <c r="G20" s="110"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="171" t="s">
+      <c r="A21" s="152" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="74">
@@ -5243,7 +5244,7 @@
         <f>SUM(C6:C20)</f>
         <v>279.56700000000001</v>
       </c>
-      <c r="D21" s="172">
+      <c r="D21" s="153">
         <f>SUM(D6:D20)</f>
         <v>6.08</v>
       </c>
@@ -5251,11 +5252,11 @@
         <f>SUM(E6:E20)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="173">
+      <c r="F21" s="154">
         <f>SUM(F6:F20)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="173">
+      <c r="G21" s="154">
         <f>SUM(B21:F21)</f>
         <v>340.27100000000002</v>
       </c>
@@ -5264,23 +5265,23 @@
       <c r="A22" s="113" t="s">
         <v>109</v>
       </c>
-      <c r="B22" s="174">
+      <c r="B22" s="155">
         <f>'Charge 08'!F4</f>
         <v>47.921999999999997</v>
       </c>
-      <c r="C22" s="156">
+      <c r="C22" s="141">
         <f>'Charge 08'!F5</f>
         <v>59.499000000000002</v>
       </c>
-      <c r="D22" s="156">
+      <c r="D22" s="141">
         <f>'Charge 08'!F6</f>
         <v>6.0789999999999997</v>
       </c>
-      <c r="E22" s="156">
+      <c r="E22" s="141">
         <f>'Charge 08'!F7</f>
         <v>0</v>
       </c>
-      <c r="F22" s="167">
+      <c r="F22" s="148">
         <f>'Charge 08'!F8</f>
         <v>0</v>
       </c>
@@ -5290,22 +5291,22 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="176" t="s">
+      <c r="A23" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="175">
+      <c r="B23" s="156">
         <f>B21-B22</f>
         <v>6.7020000000000053</v>
       </c>
-      <c r="C23" s="168">
+      <c r="C23" s="149">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
         <v>220.06800000000001</v>
       </c>
-      <c r="D23" s="168">
+      <c r="D23" s="149">
         <f t="shared" si="0"/>
         <v>1.000000000000334E-3</v>
       </c>
-      <c r="E23" s="168">
+      <c r="E23" s="149">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5320,6 +5321,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A1:G1"/>
@@ -5340,7 +5342,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5362,15 +5364,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="176" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="56" t="s">
@@ -5389,8 +5391,8 @@
     </row>
     <row r="3" spans="1:27" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="str">
-        <f>Q4 &amp; R4*100 &amp; Q5 &amp; R5*100 &amp; Q6 &amp; R6*100 &amp; Q7 &amp; R7*100 &amp; Q8 &amp; R8*100</f>
-        <v>Mg65Zn30Ca5D0E0</v>
+        <f>Q4 &amp; R4*100 &amp; IF(R5=0, "", Q5 &amp; R5*100) &amp; IF(R6=0, "", Q6 &amp; R6*100) &amp; IF(R7=0, "", Q7 &amp; R7*100) &amp; IF(R8=0, "", Q8 &amp; R8*100)</f>
+        <v>Mg65Zn30Ca5</v>
       </c>
       <c r="B3" s="58"/>
       <c r="C3" s="59" t="s">
@@ -5409,8 +5411,8 @@
         <v>23</v>
       </c>
       <c r="I3" s="64" t="str">
-        <f>Q4 &amp; ROUND(N4,3)*100 &amp; Q5 &amp; ROUND(N5,3)*100 &amp; Q6 &amp; ROUND(N6,3)*100 &amp; Q7 &amp; ROUND(N7,3)*100 &amp; Q8 &amp; ROUND(N8,3)*100</f>
-        <v>Mg33.7Zn64.1Ca2.3D0E0</v>
+        <f>Q4 &amp; ROUND(N4,3)*100 &amp; IF(N5=0, "", Q5 &amp; ROUND(N5,3)*100) &amp; IF(N6=0, "", Q6 &amp; ROUND(N6,3)*100) &amp; IF(N7=0, "", Q7 &amp; ROUND(N7,3)*100) &amp; IF(N8=0, "", Q8 &amp; ROUND(N8,3)*100)</f>
+        <v>Mg33.7Zn64.1Ca2.3</v>
       </c>
       <c r="J3" s="65"/>
       <c r="K3" s="66" t="s">
@@ -6005,35 +6007,35 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="146" t="str">
+      <c r="A12" s="180" t="str">
         <f>$Q$4</f>
         <v>Mg</v>
       </c>
-      <c r="B12" s="147"/>
+      <c r="B12" s="181"/>
       <c r="C12" s="91"/>
-      <c r="D12" s="148" t="str">
+      <c r="D12" s="182" t="str">
         <f>$Q$5</f>
         <v>Zn</v>
       </c>
-      <c r="E12" s="149"/>
+      <c r="E12" s="183"/>
       <c r="F12" s="91"/>
-      <c r="G12" s="150" t="str">
+      <c r="G12" s="184" t="str">
         <f>$Q$6</f>
         <v>Ca</v>
       </c>
-      <c r="H12" s="151"/>
+      <c r="H12" s="185"/>
       <c r="I12" s="92"/>
-      <c r="J12" s="152" t="str">
+      <c r="J12" s="188" t="str">
         <f>$Q$7</f>
         <v>D</v>
       </c>
-      <c r="K12" s="153"/>
+      <c r="K12" s="189"/>
       <c r="L12" s="91"/>
-      <c r="M12" s="154" t="str">
+      <c r="M12" s="186" t="str">
         <f>$Q$8</f>
         <v>E</v>
       </c>
-      <c r="N12" s="155"/>
+      <c r="N12" s="187"/>
       <c r="P12" s="93" t="s">
         <v>90</v>
       </c>
@@ -6068,17 +6070,17 @@
         <v>22</v>
       </c>
       <c r="I13" s="100"/>
-      <c r="J13" s="105" t="s">
+      <c r="J13" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="K13" s="106" t="s">
+      <c r="K13" s="108" t="s">
         <v>22</v>
       </c>
       <c r="L13" s="100"/>
-      <c r="M13" s="107" t="s">
+      <c r="M13" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="N13" s="108" t="s">
+      <c r="N13" s="106" t="s">
         <v>22</v>
       </c>
       <c r="P13" s="109" t="s">
@@ -6883,35 +6885,35 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:27" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="143" t="s">
+      <c r="A32" s="177" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="144"/>
-      <c r="C32" s="144"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="144"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="144"/>
-      <c r="J32" s="144"/>
-      <c r="K32" s="144"/>
-      <c r="L32" s="144"/>
-      <c r="M32" s="144"/>
-      <c r="N32" s="144"/>
-      <c r="O32" s="144"/>
-      <c r="P32" s="144"/>
-      <c r="Q32" s="144"/>
-      <c r="R32" s="144"/>
-      <c r="S32" s="144"/>
-      <c r="T32" s="144"/>
-      <c r="U32" s="144"/>
-      <c r="V32" s="144"/>
-      <c r="W32" s="144"/>
-      <c r="X32" s="144"/>
-      <c r="Y32" s="144"/>
-      <c r="Z32" s="144"/>
-      <c r="AA32" s="145"/>
+      <c r="B32" s="178"/>
+      <c r="C32" s="178"/>
+      <c r="D32" s="178"/>
+      <c r="E32" s="178"/>
+      <c r="F32" s="178"/>
+      <c r="G32" s="178"/>
+      <c r="H32" s="178"/>
+      <c r="I32" s="178"/>
+      <c r="J32" s="178"/>
+      <c r="K32" s="178"/>
+      <c r="L32" s="178"/>
+      <c r="M32" s="178"/>
+      <c r="N32" s="178"/>
+      <c r="O32" s="178"/>
+      <c r="P32" s="178"/>
+      <c r="Q32" s="178"/>
+      <c r="R32" s="178"/>
+      <c r="S32" s="178"/>
+      <c r="T32" s="178"/>
+      <c r="U32" s="178"/>
+      <c r="V32" s="178"/>
+      <c r="W32" s="178"/>
+      <c r="X32" s="178"/>
+      <c r="Y32" s="178"/>
+      <c r="Z32" s="178"/>
+      <c r="AA32" s="179"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
@@ -8216,7 +8218,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
         <v>4.7270000000000003</v>
       </c>
       <c r="D2" s="1">
@@ -8239,7 +8241,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
+        <f t="shared" si="0"/>
         <v>4.8339999999999996</v>
       </c>
       <c r="D3" s="1"/>
@@ -8259,7 +8261,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
+        <f t="shared" si="0"/>
         <v>5.4930000000000003</v>
       </c>
       <c r="D4" s="1"/>
@@ -8279,7 +8281,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>7.2839999999999998</v>
       </c>
     </row>
@@ -8291,7 +8293,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>7.6580000000000004</v>
       </c>
     </row>
@@ -8303,7 +8305,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>8.6839999999999993</v>
       </c>
     </row>
@@ -8315,7 +8317,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>9.6129999999999995</v>
       </c>
     </row>
@@ -8327,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>6.3310000000000004</v>
       </c>
     </row>
@@ -8337,7 +8339,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8347,7 +8349,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8357,7 +8359,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8367,7 +8369,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8377,7 +8379,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8387,7 +8389,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8397,7 +8399,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8407,7 +8409,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8417,7 +8419,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8427,7 +8429,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8437,7 +8439,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8447,7 +8449,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8457,7 +8459,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8467,7 +8469,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8477,7 +8479,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8487,7 +8489,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8497,7 +8499,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8507,7 +8509,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8517,7 +8519,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8527,7 +8529,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8537,7 +8539,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8547,7 +8549,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8557,7 +8559,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8567,7 +8569,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8577,7 +8579,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8587,7 +8589,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8597,7 +8599,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8607,7 +8609,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8617,7 +8619,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8627,7 +8629,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8637,7 +8639,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8647,7 +8649,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8657,7 +8659,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8667,7 +8669,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8677,7 +8679,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8687,7 +8689,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8697,7 +8699,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8707,7 +8709,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8717,7 +8719,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8727,7 +8729,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8737,7 +8739,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8747,7 +8749,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9935,6 +9937,584 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:F51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" style="136" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="136" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="54" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="130"/>
+      <c r="B2" s="130">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>SUM(C:C)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="53">
+        <f>'Charge 08'!F7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="130"/>
+      <c r="B3" s="130">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="53">
+        <f>SUM(C:C)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="130"/>
+      <c r="B4" s="130">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="53">
+        <f>F3-F2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="130"/>
+      <c r="B5" s="130">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="130"/>
+      <c r="B6" s="130">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="130"/>
+      <c r="B7" s="130">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="130"/>
+      <c r="B8" s="130">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="130"/>
+      <c r="B9" s="130">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="130"/>
+      <c r="B10" s="130">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="130"/>
+      <c r="B11" s="130">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="130"/>
+      <c r="B12" s="130">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="130"/>
+      <c r="B13" s="130">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="130"/>
+      <c r="B14" s="130">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="130"/>
+      <c r="B15" s="130">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="130"/>
+      <c r="B16" s="130">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="130"/>
+      <c r="B17" s="130">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="130"/>
+      <c r="B18" s="130">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="130"/>
+      <c r="B19" s="130">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="130"/>
+      <c r="B20" s="130">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="130"/>
+      <c r="B21" s="130">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="130"/>
+      <c r="B22" s="130">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="130"/>
+      <c r="B23" s="130">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="130"/>
+      <c r="B24" s="130">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="130"/>
+      <c r="B25" s="130">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="130"/>
+      <c r="B26" s="130">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="130"/>
+      <c r="B27" s="130">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="130"/>
+      <c r="B28" s="130">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="130"/>
+      <c r="B29" s="130">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="130"/>
+      <c r="B30" s="130">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="130"/>
+      <c r="B31" s="130">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="130"/>
+      <c r="B32" s="130">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="130"/>
+      <c r="B33" s="130">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="130"/>
+      <c r="B34" s="130">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="130"/>
+      <c r="B35" s="130">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="130"/>
+      <c r="B36" s="130">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="130"/>
+      <c r="B37" s="130">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="130"/>
+      <c r="B38" s="130">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="130"/>
+      <c r="B39" s="130">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="130"/>
+      <c r="B40" s="130">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="130"/>
+      <c r="B41" s="130">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="130"/>
+      <c r="B42" s="130">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="130"/>
+      <c r="B43" s="130">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="130"/>
+      <c r="B44" s="130">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="130"/>
+      <c r="B45" s="130">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="130"/>
+      <c r="B46" s="130">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="130"/>
+      <c r="B47" s="130">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="130"/>
+      <c r="B48" s="130">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="130"/>
+      <c r="B49" s="130">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="130"/>
+      <c r="B50" s="130">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="130"/>
+      <c r="B51" s="130">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1">
+    <sortState ref="A2:C51">
+      <sortCondition descending="1" ref="B1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:F51"/>
@@ -9968,584 +10548,6 @@
         <v>108</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="54" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="130"/>
-      <c r="B2" s="130">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <f>SUM(C:C)</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="53">
-        <f>'Charge 08'!F7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="130"/>
-      <c r="B3" s="130">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E3" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="53">
-        <f>SUM(C:C)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="130"/>
-      <c r="B4" s="130">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="53">
-        <f>F3-F2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="130"/>
-      <c r="B5" s="130">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="130"/>
-      <c r="B6" s="130">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="130"/>
-      <c r="B7" s="130">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="130"/>
-      <c r="B8" s="130">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="130"/>
-      <c r="B9" s="130">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
-      <c r="B10" s="130">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="130"/>
-      <c r="B11" s="130">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="130"/>
-      <c r="B12" s="130">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="130"/>
-      <c r="B13" s="130">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="130"/>
-      <c r="B14" s="130">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="130"/>
-      <c r="B15" s="130">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="130"/>
-      <c r="B16" s="130">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="130"/>
-      <c r="B17" s="130">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="130"/>
-      <c r="B18" s="130">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="130"/>
-      <c r="B19" s="130">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="130"/>
-      <c r="B20" s="130">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="130"/>
-      <c r="B21" s="130">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="130"/>
-      <c r="B22" s="130">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="130"/>
-      <c r="B23" s="130">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="130"/>
-      <c r="B24" s="130">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="130"/>
-      <c r="B25" s="130">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="130"/>
-      <c r="B26" s="130">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="130"/>
-      <c r="B27" s="130">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="130"/>
-      <c r="B28" s="130">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="130"/>
-      <c r="B29" s="130">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="130"/>
-      <c r="B30" s="130">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="130"/>
-      <c r="B31" s="130">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="130"/>
-      <c r="B32" s="130">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="130"/>
-      <c r="B33" s="130">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="130"/>
-      <c r="B34" s="130">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="130"/>
-      <c r="B35" s="130">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="130"/>
-      <c r="B36" s="130">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="130"/>
-      <c r="B37" s="130">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="130"/>
-      <c r="B38" s="130">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="130"/>
-      <c r="B39" s="130">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="130"/>
-      <c r="B40" s="130">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="130"/>
-      <c r="B41" s="130">
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="130"/>
-      <c r="B42" s="130">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="130"/>
-      <c r="B43" s="130">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="130"/>
-      <c r="B44" s="130">
-        <v>0</v>
-      </c>
-      <c r="C44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="130"/>
-      <c r="B45" s="130">
-        <v>0</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="130"/>
-      <c r="B46" s="130">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="130"/>
-      <c r="B47" s="130">
-        <v>0</v>
-      </c>
-      <c r="C47">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="130"/>
-      <c r="B48" s="130">
-        <v>0</v>
-      </c>
-      <c r="C48">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="130"/>
-      <c r="B49" s="130">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="130"/>
-      <c r="B50" s="130">
-        <v>0</v>
-      </c>
-      <c r="C50">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="130"/>
-      <c r="B51" s="130">
-        <v>0</v>
-      </c>
-      <c r="C51">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:C1">
-    <sortState ref="A2:C51">
-      <sortCondition descending="1" ref="B1"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:F51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.7109375" style="136" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="136" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="54" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="54" t="s">
         <v>115</v>
       </c>
       <c r="F1" s="54" t="s">

</xml_diff>

<commit_message>
Confirmed stock, and made nominal Charge 08
</commit_message>
<xml_diff>
--- a/Charge 08 - T06.xlsx
+++ b/Charge 08 - T06.xlsx
@@ -1475,6 +1475,18 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1530,28 +1542,16 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4716,43 +4716,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="170" t="str">
+      <c r="A1" s="174" t="str">
         <f>'Charge 08'!A1:G1</f>
         <v>Charge 08 - T06</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="172"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="176"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="173" t="str">
+      <c r="A2" s="177" t="str">
         <f>"Nominal  " &amp; 'Charge 08'!A3</f>
         <v>Nominal  Mg65Zn30Ca5</v>
       </c>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="175"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="179"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="173" t="str">
+      <c r="A3" s="177" t="str">
         <f>"Actual  " &amp; 'Charge 08'!I3</f>
-        <v>Actual  Mg33.7Zn64.1Ca2.3</v>
-      </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="174"/>
-      <c r="G3" s="175"/>
+        <v>Actual  Mg64.1Zn30.7Ca5.2</v>
+      </c>
+      <c r="B3" s="178"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="178"/>
+      <c r="F3" s="178"/>
+      <c r="G3" s="179"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="168" t="s">
+      <c r="A4" s="172" t="s">
         <v>172</v>
       </c>
       <c r="B4" s="140" t="str">
@@ -4767,7 +4767,7 @@
         <f>'Charge 08'!Q6</f>
         <v>Ca</v>
       </c>
-      <c r="E4" s="190" t="str">
+      <c r="E4" s="168" t="str">
         <f>'Charge 08'!Q7</f>
         <v>D</v>
       </c>
@@ -4780,7 +4780,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="169"/>
+      <c r="A5" s="173"/>
       <c r="B5" s="143" t="s">
         <v>22</v>
       </c>
@@ -4790,10 +4790,10 @@
       <c r="D5" s="145" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="191" t="s">
+      <c r="E5" s="169" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="192" t="s">
+      <c r="F5" s="170" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="160" t="s">
@@ -4806,11 +4806,11 @@
       </c>
       <c r="B6" s="109">
         <f>'Charge 08'!B14</f>
-        <v>4.7270000000000003</v>
+        <v>9.6129999999999995</v>
       </c>
       <c r="C6" s="146">
         <f>'Charge 08'!E14</f>
-        <v>15.063000000000001</v>
+        <v>12.114000000000001</v>
       </c>
       <c r="D6" s="146">
         <f>'Charge 08'!H14</f>
@@ -4826,7 +4826,7 @@
       </c>
       <c r="G6" s="161">
         <f>COUNTIF(B6:B20, "&lt;&gt;0")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H6" s="137" t="str">
         <f>B4</f>
@@ -4839,7 +4839,7 @@
       </c>
       <c r="B7" s="112">
         <f>'Charge 08'!B15</f>
-        <v>4.8339999999999996</v>
+        <v>8.6839999999999993</v>
       </c>
       <c r="C7" s="111">
         <f>'Charge 08'!E15</f>
@@ -4859,7 +4859,7 @@
       </c>
       <c r="G7" s="162">
         <f>COUNTIF(C6:C20, "&lt;&gt;0")</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H7" s="163" t="str">
         <f>C4</f>
@@ -4872,7 +4872,7 @@
       </c>
       <c r="B8" s="112">
         <f>'Charge 08'!B16</f>
-        <v>5.4930000000000003</v>
+        <v>7.6580000000000004</v>
       </c>
       <c r="C8" s="111">
         <f>'Charge 08'!E16</f>
@@ -4909,7 +4909,7 @@
       </c>
       <c r="C9" s="111">
         <f>'Charge 08'!E17</f>
-        <v>12.114000000000001</v>
+        <v>0</v>
       </c>
       <c r="D9" s="111">
         <f>'Charge 08'!H17</f>
@@ -4938,11 +4938,11 @@
       </c>
       <c r="B10" s="112">
         <f>'Charge 08'!B18</f>
-        <v>7.6580000000000004</v>
+        <v>6.3310000000000004</v>
       </c>
       <c r="C10" s="111">
         <f>'Charge 08'!E18</f>
-        <v>12.664</v>
+        <v>0</v>
       </c>
       <c r="D10" s="111">
         <f>'Charge 08'!H18</f>
@@ -4960,7 +4960,7 @@
         <f>COUNTIF(F6:F20, "&lt;&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="H10" s="193" t="str">
+      <c r="H10" s="171" t="str">
         <f>F4</f>
         <v>E</v>
       </c>
@@ -4971,11 +4971,11 @@
       </c>
       <c r="B11" s="112">
         <f>'Charge 08'!B19</f>
-        <v>8.6839999999999993</v>
+        <v>5.4930000000000003</v>
       </c>
       <c r="C11" s="111">
         <f>'Charge 08'!E19</f>
-        <v>193.78</v>
+        <v>0</v>
       </c>
       <c r="D11" s="111">
         <f>'Charge 08'!H19</f>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="G11" s="166">
         <f>COUNTIF(B6:F20, "&lt;&gt;0")</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H11" s="167" t="str">
         <f>G4</f>
@@ -5004,7 +5004,7 @@
       </c>
       <c r="B12" s="112">
         <f>'Charge 08'!B20</f>
-        <v>9.6129999999999995</v>
+        <v>0</v>
       </c>
       <c r="C12" s="111">
         <f>'Charge 08'!E20</f>
@@ -5030,7 +5030,7 @@
       </c>
       <c r="B13" s="112">
         <f>'Charge 08'!B21</f>
-        <v>6.3310000000000004</v>
+        <v>0</v>
       </c>
       <c r="C13" s="111">
         <f>'Charge 08'!E21</f>
@@ -5238,11 +5238,11 @@
       </c>
       <c r="B21" s="74">
         <f>SUM(B6:B20)</f>
-        <v>54.624000000000002</v>
+        <v>45.063000000000002</v>
       </c>
       <c r="C21" s="38">
         <f>SUM(C6:C20)</f>
-        <v>279.56700000000001</v>
+        <v>58.06</v>
       </c>
       <c r="D21" s="153">
         <f>SUM(D6:D20)</f>
@@ -5258,7 +5258,7 @@
       </c>
       <c r="G21" s="154">
         <f>SUM(B21:F21)</f>
-        <v>340.27100000000002</v>
+        <v>109.203</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5267,15 +5267,15 @@
       </c>
       <c r="B22" s="155">
         <f>'Charge 08'!F4</f>
-        <v>47.921999999999997</v>
+        <v>44.966999999999999</v>
       </c>
       <c r="C22" s="141">
         <f>'Charge 08'!F5</f>
-        <v>59.499000000000002</v>
+        <v>55.829000000000001</v>
       </c>
       <c r="D22" s="141">
         <f>'Charge 08'!F6</f>
-        <v>6.0789999999999997</v>
+        <v>5.7039999999999997</v>
       </c>
       <c r="E22" s="141">
         <f>'Charge 08'!F7</f>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="G22" s="72">
         <f>SUM(B22:F22)</f>
-        <v>113.49999999999999</v>
+        <v>106.49999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5296,15 +5296,15 @@
       </c>
       <c r="B23" s="156">
         <f>B21-B22</f>
-        <v>6.7020000000000053</v>
+        <v>9.6000000000003638E-2</v>
       </c>
       <c r="C23" s="149">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
-        <v>220.06800000000001</v>
+        <v>2.2310000000000016</v>
       </c>
       <c r="D23" s="149">
         <f t="shared" si="0"/>
-        <v>1.000000000000334E-3</v>
+        <v>0.37600000000000033</v>
       </c>
       <c r="E23" s="149">
         <f t="shared" si="0"/>
@@ -5316,7 +5316,7 @@
       </c>
       <c r="G23" s="117">
         <f t="shared" si="0"/>
-        <v>226.77100000000002</v>
+        <v>2.7030000000000172</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -5364,15 +5364,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="180" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
     </row>
     <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="56" t="s">
@@ -5412,7 +5412,7 @@
       </c>
       <c r="I3" s="64" t="str">
         <f>Q4 &amp; ROUND(N4,3)*100 &amp; IF(N5=0, "", Q5 &amp; ROUND(N5,3)*100) &amp; IF(N6=0, "", Q6 &amp; ROUND(N6,3)*100) &amp; IF(N7=0, "", Q7 &amp; ROUND(N7,3)*100) &amp; IF(N8=0, "", Q8 &amp; ROUND(N8,3)*100)</f>
-        <v>Mg33.7Zn64.1Ca2.3</v>
+        <v>Mg64.1Zn30.7Ca5.2</v>
       </c>
       <c r="J3" s="65"/>
       <c r="K3" s="66" t="s">
@@ -5484,11 +5484,11 @@
       </c>
       <c r="F4" s="71">
         <f>ROUND(E4*$F$9, 3)</f>
-        <v>47.921999999999997</v>
+        <v>44.966999999999999</v>
       </c>
       <c r="G4" s="72">
         <f>IFERROR(F4/U4, 0)</f>
-        <v>27.573072497123128</v>
+        <v>25.872842347525893</v>
       </c>
       <c r="I4" s="73" t="str">
         <f>$Q$4</f>
@@ -5497,19 +5497,19 @@
       <c r="J4" s="28"/>
       <c r="K4" s="74">
         <f>B29</f>
-        <v>54.624000000000002</v>
+        <v>45.063000000000002</v>
       </c>
       <c r="L4" s="75">
         <f>K4/$K$9</f>
-        <v>0.1605308709822465</v>
+        <v>0.41265349853026018</v>
       </c>
       <c r="M4" s="25">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>6.604849659833224E-3</v>
+        <v>1.6978132011119529E-2</v>
       </c>
       <c r="N4" s="120">
         <f>M4/$M$9</f>
-        <v>0.33669270145147684</v>
+        <v>0.64070645147734573</v>
       </c>
       <c r="P4" s="17">
         <v>1</v>
@@ -5577,11 +5577,11 @@
       </c>
       <c r="F5" s="71">
         <f>ROUND(E5*$F$9, 3)</f>
-        <v>59.499000000000002</v>
+        <v>55.829000000000001</v>
       </c>
       <c r="G5" s="72">
         <f>IFERROR(F5/U5, 0)</f>
-        <v>8.3331932773109259</v>
+        <v>7.8191876750700287</v>
       </c>
       <c r="I5" s="73" t="str">
         <f>$Q$5</f>
@@ -5590,19 +5590,19 @@
       <c r="J5" s="29"/>
       <c r="K5" s="77">
         <f>E29</f>
-        <v>279.56700000000001</v>
+        <v>58.06</v>
       </c>
       <c r="L5" s="78">
         <f>K5/$K$9</f>
-        <v>0.82160101801211383</v>
+        <v>0.53167037535598838</v>
       </c>
       <c r="M5" s="26">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>1.2566165275031564E-2</v>
+        <v>8.1317545403320236E-3</v>
       </c>
       <c r="N5" s="121">
         <f>M5/$M$9</f>
-        <v>0.64058023289555865</v>
+        <v>0.30686930649430005</v>
       </c>
       <c r="P5" s="17">
         <v>2</v>
@@ -5670,11 +5670,11 @@
       </c>
       <c r="F6" s="71">
         <f>ROUND(E6*$F$9, 3)</f>
-        <v>6.0789999999999997</v>
+        <v>5.7039999999999997</v>
       </c>
       <c r="G6" s="72">
         <f>IFERROR(F6/U6, 0)</f>
-        <v>3.9219354838709672</v>
+        <v>3.6799999999999997</v>
       </c>
       <c r="I6" s="73" t="str">
         <f>$Q$6</f>
@@ -5687,15 +5687,15 @@
       </c>
       <c r="L6" s="78">
         <f>K6/$K$9</f>
-        <v>1.7868111005639623E-2</v>
+        <v>5.5676126113751452E-2</v>
       </c>
       <c r="M6" s="26">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>4.4583340001096914E-4</v>
+        <v>1.3891942241067779E-3</v>
       </c>
       <c r="N6" s="121">
         <f>M6/$M$9</f>
-        <v>2.2727065652964524E-2</v>
+        <v>5.2424242028354204E-2</v>
       </c>
       <c r="P6" s="17">
         <v>3</v>
@@ -5947,11 +5947,11 @@
         <v>1</v>
       </c>
       <c r="F9" s="7">
-        <v>113.5</v>
+        <v>106.5</v>
       </c>
       <c r="G9" s="119">
         <f>SUM(G4:G8)</f>
-        <v>39.828201258305022</v>
+        <v>37.372030022595922</v>
       </c>
       <c r="I9" s="85"/>
       <c r="J9" s="81" t="s">
@@ -5959,7 +5959,7 @@
       </c>
       <c r="K9" s="122">
         <f>SUM(K4:K8)</f>
-        <v>340.27100000000002</v>
+        <v>109.203</v>
       </c>
       <c r="L9" s="86">
         <f>SUM(L4:L8)</f>
@@ -5967,11 +5967,11 @@
       </c>
       <c r="M9" s="123">
         <f>SUM(M4:M8)</f>
-        <v>1.9616848334875758E-2</v>
+        <v>2.6499080775558331E-2</v>
       </c>
       <c r="N9" s="87">
         <f>SUM(N4:N8)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="P9" s="17" t="s">
         <v>111</v>
@@ -6007,35 +6007,35 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="180" t="str">
+      <c r="A12" s="184" t="str">
         <f>$Q$4</f>
         <v>Mg</v>
       </c>
-      <c r="B12" s="181"/>
+      <c r="B12" s="185"/>
       <c r="C12" s="91"/>
-      <c r="D12" s="182" t="str">
+      <c r="D12" s="186" t="str">
         <f>$Q$5</f>
         <v>Zn</v>
       </c>
-      <c r="E12" s="183"/>
+      <c r="E12" s="187"/>
       <c r="F12" s="91"/>
-      <c r="G12" s="184" t="str">
+      <c r="G12" s="188" t="str">
         <f>$Q$6</f>
         <v>Ca</v>
       </c>
-      <c r="H12" s="185"/>
+      <c r="H12" s="189"/>
       <c r="I12" s="92"/>
-      <c r="J12" s="188" t="str">
+      <c r="J12" s="190" t="str">
         <f>$Q$7</f>
         <v>D</v>
       </c>
-      <c r="K12" s="189"/>
+      <c r="K12" s="191"/>
       <c r="L12" s="91"/>
-      <c r="M12" s="186" t="str">
+      <c r="M12" s="192" t="str">
         <f>$Q$8</f>
         <v>E</v>
       </c>
-      <c r="N12" s="187"/>
+      <c r="N12" s="193"/>
       <c r="P12" s="93" t="s">
         <v>90</v>
       </c>
@@ -6101,7 +6101,7 @@
       </c>
       <c r="B14" s="110">
         <f>A!C2</f>
-        <v>4.7270000000000003</v>
+        <v>9.6129999999999995</v>
       </c>
       <c r="C14" s="111"/>
       <c r="D14" s="132">
@@ -6109,7 +6109,7 @@
       </c>
       <c r="E14" s="110">
         <f>B!C2</f>
-        <v>15.063000000000001</v>
+        <v>12.114000000000001</v>
       </c>
       <c r="F14" s="111"/>
       <c r="G14" s="132">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="B15" s="110">
         <f>A!C3</f>
-        <v>4.8339999999999996</v>
+        <v>8.6839999999999993</v>
       </c>
       <c r="C15" s="111"/>
       <c r="D15" s="132">
@@ -6205,7 +6205,7 @@
       </c>
       <c r="B16" s="110">
         <f>A!C4</f>
-        <v>5.4930000000000003</v>
+        <v>7.6580000000000004</v>
       </c>
       <c r="C16" s="111"/>
       <c r="D16" s="132">
@@ -6265,7 +6265,7 @@
       </c>
       <c r="E17" s="110">
         <f>B!C5</f>
-        <v>12.114000000000001</v>
+        <v>0</v>
       </c>
       <c r="F17" s="111"/>
       <c r="G17" s="132">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="B18" s="110">
         <f>A!C6</f>
-        <v>7.6580000000000004</v>
+        <v>6.3310000000000004</v>
       </c>
       <c r="C18" s="111"/>
       <c r="D18" s="132">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="E18" s="110">
         <f>B!C6</f>
-        <v>12.664</v>
+        <v>0</v>
       </c>
       <c r="F18" s="111"/>
       <c r="G18" s="132">
@@ -6363,7 +6363,7 @@
       </c>
       <c r="B19" s="110">
         <f>A!C7</f>
-        <v>8.6839999999999993</v>
+        <v>5.4930000000000003</v>
       </c>
       <c r="C19" s="111"/>
       <c r="D19" s="132">
@@ -6371,7 +6371,7 @@
       </c>
       <c r="E19" s="110">
         <f>B!C7</f>
-        <v>193.78</v>
+        <v>0</v>
       </c>
       <c r="F19" s="111"/>
       <c r="G19" s="132">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="B20" s="110">
         <f>A!C8</f>
-        <v>9.6129999999999995</v>
+        <v>0</v>
       </c>
       <c r="C20" s="111"/>
       <c r="D20" s="132">
@@ -6463,7 +6463,7 @@
       </c>
       <c r="B21" s="110">
         <f>A!C9</f>
-        <v>6.3310000000000004</v>
+        <v>0</v>
       </c>
       <c r="C21" s="111"/>
       <c r="D21" s="132">
@@ -6807,7 +6807,7 @@
       </c>
       <c r="B29" s="114">
         <f>SUM(B14:B28)</f>
-        <v>54.624000000000002</v>
+        <v>45.063000000000002</v>
       </c>
       <c r="C29" s="111"/>
       <c r="D29" s="113" t="s">
@@ -6815,7 +6815,7 @@
       </c>
       <c r="E29" s="115">
         <f>SUM(E14:E28)</f>
-        <v>279.56700000000001</v>
+        <v>58.06</v>
       </c>
       <c r="F29" s="111"/>
       <c r="G29" s="113" t="s">
@@ -6848,7 +6848,7 @@
       </c>
       <c r="B30" s="117">
         <f>B29-$F$4</f>
-        <v>6.7020000000000053</v>
+        <v>9.6000000000003638E-2</v>
       </c>
       <c r="C30" s="118"/>
       <c r="D30" s="116" t="s">
@@ -6856,7 +6856,7 @@
       </c>
       <c r="E30" s="117">
         <f>E29-$F$5</f>
-        <v>220.06800000000001</v>
+        <v>2.2310000000000016</v>
       </c>
       <c r="F30" s="118"/>
       <c r="G30" s="116" t="s">
@@ -6864,7 +6864,7 @@
       </c>
       <c r="H30" s="117">
         <f>H29-$F$6</f>
-        <v>1.000000000000334E-3</v>
+        <v>0.37600000000000033</v>
       </c>
       <c r="I30" s="118"/>
       <c r="J30" s="116" t="s">
@@ -6885,35 +6885,35 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:27" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="177" t="s">
+      <c r="A32" s="181" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="178"/>
-      <c r="C32" s="178"/>
-      <c r="D32" s="178"/>
-      <c r="E32" s="178"/>
-      <c r="F32" s="178"/>
-      <c r="G32" s="178"/>
-      <c r="H32" s="178"/>
-      <c r="I32" s="178"/>
-      <c r="J32" s="178"/>
-      <c r="K32" s="178"/>
-      <c r="L32" s="178"/>
-      <c r="M32" s="178"/>
-      <c r="N32" s="178"/>
-      <c r="O32" s="178"/>
-      <c r="P32" s="178"/>
-      <c r="Q32" s="178"/>
-      <c r="R32" s="178"/>
-      <c r="S32" s="178"/>
-      <c r="T32" s="178"/>
-      <c r="U32" s="178"/>
-      <c r="V32" s="178"/>
-      <c r="W32" s="178"/>
-      <c r="X32" s="178"/>
-      <c r="Y32" s="178"/>
-      <c r="Z32" s="178"/>
-      <c r="AA32" s="179"/>
+      <c r="B32" s="182"/>
+      <c r="C32" s="182"/>
+      <c r="D32" s="182"/>
+      <c r="E32" s="182"/>
+      <c r="F32" s="182"/>
+      <c r="G32" s="182"/>
+      <c r="H32" s="182"/>
+      <c r="I32" s="182"/>
+      <c r="J32" s="182"/>
+      <c r="K32" s="182"/>
+      <c r="L32" s="182"/>
+      <c r="M32" s="182"/>
+      <c r="N32" s="182"/>
+      <c r="O32" s="182"/>
+      <c r="P32" s="182"/>
+      <c r="Q32" s="182"/>
+      <c r="R32" s="182"/>
+      <c r="S32" s="182"/>
+      <c r="T32" s="182"/>
+      <c r="U32" s="182"/>
+      <c r="V32" s="182"/>
+      <c r="W32" s="182"/>
+      <c r="X32" s="182"/>
+      <c r="Y32" s="182"/>
+      <c r="Z32" s="182"/>
+      <c r="AA32" s="183"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
@@ -8211,38 +8211,38 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="130">
-        <v>4.7270000000000003</v>
+      <c r="A2" s="131">
+        <v>9.6129999999999995</v>
       </c>
       <c r="B2" s="130">
         <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>4.7270000000000003</v>
+        <f>IF(A2=0, 0, A2*B2)</f>
+        <v>9.6129999999999995</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>54.624000000000002</v>
+        <v>45.063000000000002</v>
       </c>
       <c r="E2" s="133" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="135">
         <f>'Charge 08'!F4</f>
-        <v>47.921999999999997</v>
+        <v>44.966999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="131">
-        <v>4.8339999999999996</v>
+      <c r="A3" s="130">
+        <v>8.6839999999999993</v>
       </c>
       <c r="B3" s="130">
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>4.8339999999999996</v>
+        <f>IF(A3=0, 0, A3*B3)</f>
+        <v>8.6839999999999993</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="133" t="s">
@@ -8250,19 +8250,19 @@
       </c>
       <c r="F3" s="135">
         <f>SUM(C:C)</f>
-        <v>54.624000000000002</v>
+        <v>45.063000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="131">
-        <v>5.4930000000000003</v>
+      <c r="A4" s="130">
+        <v>7.6580000000000004</v>
       </c>
       <c r="B4" s="130">
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>5.4930000000000003</v>
+        <f>IF(A4=0, 0, A4*B4)</f>
+        <v>7.6580000000000004</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="133" t="s">
@@ -8270,7 +8270,7 @@
       </c>
       <c r="F4" s="135">
         <f>F3-F2</f>
-        <v>6.7020000000000053</v>
+        <v>9.6000000000003638E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8281,56 +8281,56 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f>IF(A5=0, 0, A5*B5)</f>
         <v>7.2839999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="130">
-        <v>7.6580000000000004</v>
+      <c r="A6" s="131">
+        <v>6.3310000000000004</v>
       </c>
       <c r="B6" s="130">
         <v>1</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>7.6580000000000004</v>
+        <f>IF(A6=0, 0, A6*B6)</f>
+        <v>6.3310000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="130">
-        <v>8.6839999999999993</v>
+      <c r="A7" s="131">
+        <v>5.4930000000000003</v>
       </c>
       <c r="B7" s="130">
         <v>1</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>8.6839999999999993</v>
+        <f>IF(A7=0, 0, A7*B7)</f>
+        <v>5.4930000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="131">
-        <v>9.6129999999999995</v>
+        <v>4.8339999999999996</v>
       </c>
       <c r="B8" s="130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>9.6129999999999995</v>
+        <f>IF(A8=0, 0, A8*B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="131">
-        <v>6.3310000000000004</v>
+      <c r="A9" s="130">
+        <v>4.7270000000000003</v>
       </c>
       <c r="B9" s="130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>6.3310000000000004</v>
+        <f>IF(A9=0, 0, A9*B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -8339,7 +8339,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
@@ -8349,7 +8349,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
@@ -8359,7 +8359,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
@@ -8369,7 +8369,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
@@ -8379,7 +8379,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
@@ -8389,7 +8389,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
@@ -8399,7 +8399,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
@@ -8409,7 +8409,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
@@ -8419,7 +8419,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
@@ -8429,7 +8429,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
@@ -8439,7 +8439,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
@@ -8449,7 +8449,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
@@ -8459,7 +8459,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
@@ -8469,7 +8469,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
@@ -8479,7 +8479,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
@@ -8489,7 +8489,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
@@ -8499,7 +8499,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
@@ -8509,7 +8509,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -8519,7 +8519,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -8529,7 +8529,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -8539,7 +8539,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -8549,7 +8549,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -8559,7 +8559,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -8569,7 +8569,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -8579,7 +8579,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8589,7 +8589,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -8599,7 +8599,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -8609,7 +8609,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -8619,7 +8619,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -8629,7 +8629,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -8639,7 +8639,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -8649,7 +8649,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -8659,7 +8659,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -8669,7 +8669,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -8679,7 +8679,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -8689,7 +8689,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -8699,7 +8699,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -8709,7 +8709,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -8719,7 +8719,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -8729,7 +8729,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -8739,7 +8739,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -8749,14 +8749,14 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition descending="1" ref="B1"/>
+      <sortCondition descending="1" ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8808,25 +8808,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="130">
-        <v>15.063000000000001</v>
+        <v>12.114000000000001</v>
       </c>
       <c r="B2" s="130">
         <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>15.063000000000001</v>
+        <f>IF(A2=0, 0, A2*B2)</f>
+        <v>12.114000000000001</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>279.56700000000001</v>
+        <v>58.06</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="53">
         <f>'Charge 08'!F5</f>
-        <v>59.499000000000002</v>
+        <v>55.829000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8837,7 +8837,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f>IF(A3=0, 0, A3*B3)</f>
         <v>16.469000000000001</v>
       </c>
       <c r="E3" s="52" t="s">
@@ -8845,7 +8845,7 @@
       </c>
       <c r="F3" s="53">
         <f>SUM(C:C)</f>
-        <v>279.56700000000001</v>
+        <v>58.06</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -8856,7 +8856,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f>IF(A4=0, 0, A4*B4)</f>
         <v>29.477</v>
       </c>
       <c r="E4" s="52" t="s">
@@ -8864,31 +8864,31 @@
       </c>
       <c r="F4" s="53">
         <f>F3-F2</f>
-        <v>220.06800000000001</v>
+        <v>2.2310000000000016</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="130">
-        <v>12.114000000000001</v>
+        <v>12.664</v>
       </c>
       <c r="B5" s="130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>12.114000000000001</v>
+        <f>IF(A5=0, 0, A5*B5)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="130">
-        <v>12.664</v>
+        <v>15.063000000000001</v>
       </c>
       <c r="B6" s="130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>12.664</v>
+        <f>IF(A6=0, 0, A6*B6)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8896,11 +8896,11 @@
         <v>193.78</v>
       </c>
       <c r="B7" s="130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>193.78</v>
+        <f>IF(A7=0, 0, A7*B7)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8909,7 +8909,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
@@ -8919,7 +8919,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
@@ -8929,7 +8929,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
@@ -8939,7 +8939,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
@@ -8949,7 +8949,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
@@ -8959,7 +8959,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
@@ -8969,7 +8969,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
@@ -8979,7 +8979,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
@@ -8989,7 +8989,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
@@ -8999,7 +8999,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
@@ -9009,7 +9009,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
@@ -9019,7 +9019,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
@@ -9029,7 +9029,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
@@ -9039,7 +9039,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
@@ -9049,7 +9049,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
@@ -9059,7 +9059,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
@@ -9069,7 +9069,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
@@ -9079,7 +9079,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
@@ -9089,7 +9089,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
@@ -9099,7 +9099,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -9109,7 +9109,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -9119,7 +9119,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -9129,7 +9129,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -9139,7 +9139,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -9149,7 +9149,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -9159,7 +9159,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -9169,7 +9169,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9179,7 +9179,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -9189,7 +9189,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -9199,7 +9199,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -9209,7 +9209,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -9219,7 +9219,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -9229,7 +9229,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -9239,7 +9239,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -9249,7 +9249,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -9259,7 +9259,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -9269,7 +9269,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -9279,7 +9279,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -9289,7 +9289,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -9299,7 +9299,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -9309,7 +9309,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -9319,7 +9319,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -9329,7 +9329,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -9339,7 +9339,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
@@ -9416,7 +9416,7 @@
       </c>
       <c r="F2" s="53">
         <f>'Charge 08'!F6</f>
-        <v>6.0789999999999997</v>
+        <v>5.7039999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9450,7 +9450,7 @@
       </c>
       <c r="F4" s="53">
         <f>F3-F2</f>
-        <v>1.000000000000334E-3</v>
+        <v>0.37600000000000033</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add more Zn pieces, add Al & Cu heat capacity Cp
</commit_message>
<xml_diff>
--- a/Charge 08 - T06.xlsx
+++ b/Charge 08 - T06.xlsx
@@ -1509,6 +1509,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1576,10 +1580,6 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2344,7 +2344,9 @@
       <c r="F14" s="1">
         <v>2519</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="2">
+        <v>900</v>
+      </c>
       <c r="H14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2866,7 +2868,9 @@
       <c r="F30" s="1">
         <v>2562</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="2">
+        <v>385</v>
+      </c>
       <c r="H30" s="2" t="s">
         <v>10</v>
       </c>
@@ -4851,43 +4855,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="170" t="str">
+      <c r="A1" s="172" t="str">
         <f>'Charge 08'!A1:G1</f>
         <v>Charge 08 - T06</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="172"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="174"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="173" t="str">
+      <c r="A2" s="175" t="str">
         <f>"Nominal  " &amp; 'Charge 08'!A3</f>
         <v>Nominal  Mg65Zn30Ca5</v>
       </c>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="175"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="177"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="173" t="str">
+      <c r="A3" s="175" t="str">
         <f>"Actual  " &amp; 'Charge 08'!I3</f>
-        <v>Actual  Mg64.1Zn30.7Ca5.2</v>
-      </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="174"/>
-      <c r="G3" s="175"/>
+        <v>Actual  Mg63.7Zn31.1Ca5.2</v>
+      </c>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
+      <c r="F3" s="176"/>
+      <c r="G3" s="177"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="168" t="s">
+      <c r="A4" s="170" t="s">
         <v>171</v>
       </c>
       <c r="B4" s="135" t="str">
@@ -4915,7 +4919,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="169"/>
+      <c r="A5" s="171"/>
       <c r="B5" s="138" t="s">
         <v>22</v>
       </c>
@@ -4945,7 +4949,7 @@
       </c>
       <c r="C6" s="141">
         <f>'Charge 08'!E14</f>
-        <v>12.114000000000001</v>
+        <v>20.94</v>
       </c>
       <c r="D6" s="141">
         <f>'Charge 08'!H14</f>
@@ -4978,7 +4982,7 @@
       </c>
       <c r="C7" s="107">
         <f>'Charge 08'!E15</f>
-        <v>16.469000000000001</v>
+        <v>13.51</v>
       </c>
       <c r="D7" s="107">
         <f>'Charge 08'!H15</f>
@@ -4994,7 +4998,7 @@
       </c>
       <c r="G7" s="157">
         <f>COUNTIF(C6:C20, "&lt;&gt;0")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H7" s="158" t="str">
         <f>C4</f>
@@ -5011,7 +5015,7 @@
       </c>
       <c r="C8" s="107">
         <f>'Charge 08'!E16</f>
-        <v>29.477</v>
+        <v>12.664</v>
       </c>
       <c r="D8" s="107">
         <f>'Charge 08'!H16</f>
@@ -5044,7 +5048,7 @@
       </c>
       <c r="C9" s="107">
         <f>'Charge 08'!E17</f>
-        <v>0</v>
+        <v>12.114000000000001</v>
       </c>
       <c r="D9" s="107">
         <f>'Charge 08'!H17</f>
@@ -5126,7 +5130,7 @@
       </c>
       <c r="G11" s="161">
         <f>COUNTIF(B6:F20, "&lt;&gt;0")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11" s="162" t="str">
         <f>G4</f>
@@ -5377,7 +5381,7 @@
       </c>
       <c r="C21" s="36">
         <f>SUM(C6:C20)</f>
-        <v>58.06</v>
+        <v>59.228000000000009</v>
       </c>
       <c r="D21" s="148">
         <f>SUM(D6:D20)</f>
@@ -5393,7 +5397,7 @@
       </c>
       <c r="G21" s="149">
         <f>SUM(B21:F21)</f>
-        <v>109.203</v>
+        <v>110.37100000000001</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5435,7 +5439,7 @@
       </c>
       <c r="C23" s="144">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
-        <v>-1.1769999999999996</v>
+        <v>-8.9999999999932356E-3</v>
       </c>
       <c r="D23" s="144">
         <f t="shared" si="0"/>
@@ -5451,7 +5455,7 @@
       </c>
       <c r="G23" s="113">
         <f t="shared" si="0"/>
-        <v>-3.796999999999997</v>
+        <v>-2.6289999999999907</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -5499,15 +5503,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="178" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
     </row>
     <row r="2" spans="1:28" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="54" t="s">
@@ -5547,7 +5551,7 @@
       </c>
       <c r="I3" s="62" t="str">
         <f>Q4 &amp; ROUND(N4,3)*100 &amp; IF(N5=0, "", Q5 &amp; ROUND(N5,3)*100) &amp; IF(N6=0, "", Q6 &amp; ROUND(N6,3)*100) &amp; IF(N7=0, "", Q7 &amp; ROUND(N7,3)*100) &amp; IF(N8=0, "", Q8 &amp; ROUND(N8,3)*100)</f>
-        <v>Mg64.1Zn30.7Ca5.2</v>
+        <v>Mg63.7Zn31.1Ca5.2</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="s">
@@ -5657,15 +5661,15 @@
       </c>
       <c r="L4" s="73">
         <f>K4/$K$9</f>
-        <v>0.41265349853026018</v>
+        <v>0.40828659702276865</v>
       </c>
       <c r="M4" s="23">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>1.6978132011119529E-2</v>
+        <v>1.6798461099476185E-2</v>
       </c>
       <c r="N4" s="115">
         <f>M4/$M$9</f>
-        <v>0.64070645147734573</v>
+        <v>0.63677542870187764</v>
       </c>
       <c r="P4" s="15">
         <v>1</v>
@@ -5750,19 +5754,19 @@
       <c r="J5" s="27"/>
       <c r="K5" s="75">
         <f>E29</f>
-        <v>58.06</v>
+        <v>59.228000000000009</v>
       </c>
       <c r="L5" s="76">
         <f>K5/$K$9</f>
-        <v>0.53167037535598838</v>
+        <v>0.53662646890940557</v>
       </c>
       <c r="M5" s="24">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>8.1317545403320236E-3</v>
+        <v>8.2075566502922137E-3</v>
       </c>
       <c r="N5" s="116">
         <f>M5/$M$9</f>
-        <v>0.30686930649430005</v>
+        <v>0.31112197561642962</v>
       </c>
       <c r="P5" s="15">
         <v>2</v>
@@ -5851,15 +5855,15 @@
       </c>
       <c r="L6" s="76">
         <f>K6/$K$9</f>
-        <v>5.5676126113751452E-2</v>
+        <v>5.5086934067825784E-2</v>
       </c>
       <c r="M6" s="24">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>1.3891942241067779E-3</v>
+        <v>1.3744930901698133E-3</v>
       </c>
       <c r="N6" s="116">
         <f>M6/$M$9</f>
-        <v>5.2424242028354204E-2</v>
+        <v>5.2102595681692745E-2</v>
       </c>
       <c r="P6" s="15">
         <v>3</v>
@@ -6122,7 +6126,7 @@
         <f>SUM(E4:E8)</f>
         <v>1</v>
       </c>
-      <c r="F9" s="190">
+      <c r="F9" s="168">
         <v>113</v>
       </c>
       <c r="G9" s="149">
@@ -6135,7 +6139,7 @@
       </c>
       <c r="K9" s="117">
         <f>SUM(K4:K8)</f>
-        <v>109.203</v>
+        <v>110.37100000000001</v>
       </c>
       <c r="L9" s="83">
         <f>SUM(L4:L8)</f>
@@ -6143,11 +6147,11 @@
       </c>
       <c r="M9" s="118">
         <f>SUM(M4:M8)</f>
-        <v>2.6499080775558331E-2</v>
+        <v>2.6380510839938212E-2</v>
       </c>
       <c r="N9" s="84">
         <f>SUM(N4:N8)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>111</v>
@@ -6181,7 +6185,7 @@
       <c r="AB9" s="146"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="F10" s="191">
+      <c r="F10" s="169">
         <f>G10*U9</f>
         <v>0</v>
       </c>
@@ -6198,35 +6202,35 @@
       </c>
     </row>
     <row r="12" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="180" t="str">
+      <c r="A12" s="182" t="str">
         <f>$Q$4</f>
         <v>Mg</v>
       </c>
-      <c r="B12" s="181"/>
+      <c r="B12" s="183"/>
       <c r="C12" s="87"/>
-      <c r="D12" s="182" t="str">
+      <c r="D12" s="184" t="str">
         <f>$Q$5</f>
         <v>Zn</v>
       </c>
-      <c r="E12" s="183"/>
+      <c r="E12" s="185"/>
       <c r="F12" s="87"/>
-      <c r="G12" s="184" t="str">
+      <c r="G12" s="186" t="str">
         <f>$Q$6</f>
         <v>Ca</v>
       </c>
-      <c r="H12" s="185"/>
+      <c r="H12" s="187"/>
       <c r="I12" s="88"/>
-      <c r="J12" s="186" t="str">
+      <c r="J12" s="188" t="str">
         <f>$Q$7</f>
         <v>D</v>
       </c>
-      <c r="K12" s="187"/>
+      <c r="K12" s="189"/>
       <c r="L12" s="87"/>
-      <c r="M12" s="188" t="str">
+      <c r="M12" s="190" t="str">
         <f>$Q$8</f>
         <v>E</v>
       </c>
-      <c r="N12" s="189"/>
+      <c r="N12" s="191"/>
       <c r="P12" s="89" t="s">
         <v>90</v>
       </c>
@@ -6300,7 +6304,7 @@
       </c>
       <c r="E14" s="106">
         <f>B!C2</f>
-        <v>12.114000000000001</v>
+        <v>20.94</v>
       </c>
       <c r="F14" s="107"/>
       <c r="G14" s="127">
@@ -6353,7 +6357,7 @@
       </c>
       <c r="E15" s="106">
         <f>B!C3</f>
-        <v>16.469000000000001</v>
+        <v>13.51</v>
       </c>
       <c r="F15" s="107"/>
       <c r="G15" s="127">
@@ -6406,7 +6410,7 @@
       </c>
       <c r="E16" s="106">
         <f>B!C4</f>
-        <v>29.477</v>
+        <v>12.664</v>
       </c>
       <c r="F16" s="107"/>
       <c r="G16" s="127">
@@ -6459,7 +6463,7 @@
       </c>
       <c r="E17" s="106">
         <f>B!C5</f>
-        <v>0</v>
+        <v>12.114000000000001</v>
       </c>
       <c r="F17" s="107"/>
       <c r="G17" s="127">
@@ -7014,7 +7018,7 @@
       </c>
       <c r="E29" s="111">
         <f>SUM(E14:E28)</f>
-        <v>58.06</v>
+        <v>59.228000000000009</v>
       </c>
       <c r="F29" s="107"/>
       <c r="G29" s="109" t="s">
@@ -7055,7 +7059,7 @@
       </c>
       <c r="E30" s="113">
         <f>E29-$F$5</f>
-        <v>-1.1769999999999996</v>
+        <v>-8.9999999999932356E-3</v>
       </c>
       <c r="F30" s="114"/>
       <c r="G30" s="112" t="s">
@@ -7084,36 +7088,36 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="177" t="s">
+      <c r="A32" s="179" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="178"/>
-      <c r="C32" s="178"/>
-      <c r="D32" s="178"/>
-      <c r="E32" s="178"/>
-      <c r="F32" s="178"/>
-      <c r="G32" s="178"/>
-      <c r="H32" s="178"/>
-      <c r="I32" s="178"/>
-      <c r="J32" s="178"/>
-      <c r="K32" s="178"/>
-      <c r="L32" s="178"/>
-      <c r="M32" s="178"/>
-      <c r="N32" s="178"/>
-      <c r="O32" s="178"/>
-      <c r="P32" s="178"/>
-      <c r="Q32" s="178"/>
-      <c r="R32" s="178"/>
-      <c r="S32" s="178"/>
-      <c r="T32" s="178"/>
-      <c r="U32" s="178"/>
-      <c r="V32" s="178"/>
-      <c r="W32" s="178"/>
-      <c r="X32" s="178"/>
-      <c r="Y32" s="178"/>
-      <c r="Z32" s="178"/>
-      <c r="AA32" s="178"/>
-      <c r="AB32" s="179"/>
+      <c r="B32" s="180"/>
+      <c r="C32" s="180"/>
+      <c r="D32" s="180"/>
+      <c r="E32" s="180"/>
+      <c r="F32" s="180"/>
+      <c r="G32" s="180"/>
+      <c r="H32" s="180"/>
+      <c r="I32" s="180"/>
+      <c r="J32" s="180"/>
+      <c r="K32" s="180"/>
+      <c r="L32" s="180"/>
+      <c r="M32" s="180"/>
+      <c r="N32" s="180"/>
+      <c r="O32" s="180"/>
+      <c r="P32" s="180"/>
+      <c r="Q32" s="180"/>
+      <c r="R32" s="180"/>
+      <c r="S32" s="180"/>
+      <c r="T32" s="180"/>
+      <c r="U32" s="180"/>
+      <c r="V32" s="180"/>
+      <c r="W32" s="180"/>
+      <c r="X32" s="180"/>
+      <c r="Y32" s="180"/>
+      <c r="Z32" s="180"/>
+      <c r="AA32" s="180"/>
+      <c r="AB32" s="181"/>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="42"/>
@@ -8460,7 +8464,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
+        <f>IF(A2=0, 0, A2*B2)</f>
         <v>9.6129999999999995</v>
       </c>
       <c r="D2" s="1">
@@ -8483,7 +8487,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f>IF(A3=0, 0, A3*B3)</f>
         <v>8.6839999999999993</v>
       </c>
       <c r="D3" s="1"/>
@@ -8503,7 +8507,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f>IF(A4=0, 0, A4*B4)</f>
         <v>7.6580000000000004</v>
       </c>
       <c r="D4" s="1"/>
@@ -8523,7 +8527,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f>IF(A5=0, 0, A5*B5)</f>
         <v>7.2839999999999998</v>
       </c>
     </row>
@@ -8535,7 +8539,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>IF(A6=0, 0, A6*B6)</f>
         <v>6.3310000000000004</v>
       </c>
     </row>
@@ -8547,7 +8551,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>IF(A7=0, 0, A7*B7)</f>
         <v>5.4930000000000003</v>
       </c>
     </row>
@@ -8559,7 +8563,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
@@ -8571,7 +8575,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
@@ -8581,7 +8585,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
@@ -8591,7 +8595,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
@@ -8601,7 +8605,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
@@ -8611,7 +8615,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
@@ -8621,7 +8625,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
@@ -8631,7 +8635,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
@@ -8641,7 +8645,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
@@ -8651,7 +8655,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
@@ -8661,7 +8665,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
@@ -8671,7 +8675,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
@@ -8681,7 +8685,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
@@ -8691,7 +8695,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
@@ -8701,7 +8705,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
@@ -8711,7 +8715,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
@@ -8721,7 +8725,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
@@ -8731,7 +8735,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
@@ -8741,7 +8745,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
@@ -8751,7 +8755,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -8761,7 +8765,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -8771,7 +8775,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -8781,7 +8785,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -8791,7 +8795,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -8801,7 +8805,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -8811,7 +8815,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -8821,7 +8825,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8831,7 +8835,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -8841,7 +8845,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -8851,7 +8855,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -8861,7 +8865,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -8871,7 +8875,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -8881,7 +8885,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -8891,7 +8895,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -8901,7 +8905,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -8911,7 +8915,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -8921,7 +8925,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -8931,7 +8935,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -8941,7 +8945,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -8951,7 +8955,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -8961,7 +8965,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -8971,7 +8975,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -8981,7 +8985,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -8991,7 +8995,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
@@ -9050,18 +9054,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>12.114000000000001</v>
+        <v>20.94</v>
       </c>
       <c r="B2" s="125">
         <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>12.114000000000001</v>
+        <f>IF(A2=0, 0, A2*B2)</f>
+        <v>20.94</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>58.06</v>
+        <v>59.228000000000009</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
@@ -9073,155 +9077,171 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="125">
-        <v>16.469000000000001</v>
+        <v>13.51</v>
       </c>
       <c r="B3" s="125">
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>16.469000000000001</v>
+        <f>IF(A3=0, 0, A3*B3)</f>
+        <v>13.51</v>
       </c>
       <c r="E3" s="50" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>58.06</v>
+        <v>59.228000000000009</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="125">
-        <v>29.477</v>
+        <v>12.664</v>
       </c>
       <c r="B4" s="125">
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>29.477</v>
+        <f>IF(A4=0, 0, A4*B4)</f>
+        <v>12.664</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-1.1769999999999996</v>
+        <v>-8.9999999999932356E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="125">
-        <v>12.664</v>
+        <v>12.114000000000001</v>
       </c>
       <c r="B5" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(A5=0, 0, A5*B5)</f>
+        <v>12.114000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="125">
-        <v>15.063000000000001</v>
+        <v>29.477</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>IF(A6=0, 0, A6*B6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="125">
-        <v>193.78</v>
+        <v>21.95</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>IF(A7=0, 0, A7*B7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="125"/>
+      <c r="A8" s="125">
+        <v>20.87</v>
+      </c>
       <c r="B8" s="125">
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="125"/>
+      <c r="A9" s="125">
+        <v>20.75</v>
+      </c>
       <c r="B9" s="125">
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="125"/>
+      <c r="A10" s="125">
+        <v>20.52</v>
+      </c>
       <c r="B10" s="125">
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="125"/>
+      <c r="A11" s="125">
+        <v>18.03</v>
+      </c>
       <c r="B11" s="125">
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="125"/>
+      <c r="A12" s="125">
+        <v>16.469000000000001</v>
+      </c>
       <c r="B12" s="125">
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
+      <c r="A13" s="125">
+        <v>15.063000000000001</v>
+      </c>
       <c r="B13" s="125">
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="125"/>
+      <c r="A14" s="125">
+        <v>14.66</v>
+      </c>
       <c r="B14" s="125">
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="125"/>
+      <c r="A15" s="125">
+        <v>12.9</v>
+      </c>
       <c r="B15" s="125">
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
@@ -9231,7 +9251,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
@@ -9241,7 +9261,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
@@ -9251,7 +9271,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
@@ -9261,7 +9281,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
@@ -9271,7 +9291,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
@@ -9281,7 +9301,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
@@ -9291,7 +9311,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
@@ -9301,7 +9321,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
@@ -9311,7 +9331,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
@@ -9321,7 +9341,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
@@ -9331,7 +9351,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
@@ -9341,7 +9361,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -9351,7 +9371,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -9361,7 +9381,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -9371,7 +9391,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -9381,7 +9401,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -9391,7 +9411,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -9401,7 +9421,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -9411,7 +9431,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9421,7 +9441,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -9431,7 +9451,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -9441,7 +9461,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -9451,7 +9471,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -9461,7 +9481,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -9471,7 +9491,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -9481,7 +9501,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -9491,7 +9511,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -9501,7 +9521,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -9511,7 +9531,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -9521,7 +9541,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -9531,7 +9551,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -9541,7 +9561,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -9551,7 +9571,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -9561,7 +9581,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -9571,7 +9591,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -9581,7 +9601,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Min/Max atomic ratio summary to alloy table
</commit_message>
<xml_diff>
--- a/Charge 08 - T06.xlsx
+++ b/Charge 08 - T06.xlsx
@@ -1186,7 +1186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1580,6 +1580,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6180,8 +6181,14 @@
         <v>812.5</v>
       </c>
       <c r="Y9" s="114"/>
-      <c r="Z9" s="114"/>
-      <c r="AA9" s="114"/>
+      <c r="Z9" s="192">
+        <f>(MAX(Z4:Z8)-SMALL(Z4:Z8,COUNTIF(Z4:Z8,"&lt;=0")+1))/MAX(Z4:Z8)</f>
+        <v>0.16874999999999998</v>
+      </c>
+      <c r="AA9" s="192">
+        <f>(MAX(AA4:AA8)-SMALL(AA4:AA8,COUNTIF(AA4:AA8,"&lt;=0")+1))/MAX(AA4:AA8)</f>
+        <v>0.2421052631578948</v>
+      </c>
       <c r="AB9" s="146"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -8399,7 +8406,6 @@
     <row r="92" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="93" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A32:AB32"/>
@@ -8464,7 +8470,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
         <v>9.6129999999999995</v>
       </c>
       <c r="D2" s="1">
@@ -8487,7 +8493,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
+        <f t="shared" si="0"/>
         <v>8.6839999999999993</v>
       </c>
       <c r="D3" s="1"/>
@@ -8507,7 +8513,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
+        <f t="shared" si="0"/>
         <v>7.6580000000000004</v>
       </c>
       <c r="D4" s="1"/>
@@ -8527,7 +8533,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>7.2839999999999998</v>
       </c>
     </row>
@@ -8539,7 +8545,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>6.3310000000000004</v>
       </c>
     </row>
@@ -8551,7 +8557,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>5.4930000000000003</v>
       </c>
     </row>
@@ -8563,7 +8569,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8575,7 +8581,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8585,7 +8591,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8595,7 +8601,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8605,7 +8611,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8615,7 +8621,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8625,7 +8631,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8635,7 +8641,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8645,7 +8651,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8655,7 +8661,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8665,7 +8671,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8675,7 +8681,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8685,7 +8691,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8695,7 +8701,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8705,7 +8711,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8715,7 +8721,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8725,7 +8731,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8735,7 +8741,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8745,7 +8751,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8755,7 +8761,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8765,7 +8771,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8775,7 +8781,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8785,7 +8791,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8795,7 +8801,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8805,7 +8811,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8815,7 +8821,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8825,7 +8831,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8835,7 +8841,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8845,7 +8851,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8855,7 +8861,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8865,7 +8871,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8875,7 +8881,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8885,7 +8891,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8895,7 +8901,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8905,7 +8911,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8915,7 +8921,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8925,7 +8931,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8935,7 +8941,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8945,7 +8951,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8955,7 +8961,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8965,7 +8971,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8975,7 +8981,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8985,7 +8991,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8995,7 +9001,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9060,7 +9066,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
         <v>20.94</v>
       </c>
       <c r="D2">
@@ -9083,7 +9089,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
+        <f t="shared" si="0"/>
         <v>13.51</v>
       </c>
       <c r="E3" s="50" t="s">
@@ -9102,7 +9108,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
+        <f t="shared" si="0"/>
         <v>12.664</v>
       </c>
       <c r="E4" s="50" t="s">
@@ -9121,7 +9127,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>12.114000000000001</v>
       </c>
     </row>
@@ -9133,7 +9139,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9145,7 +9151,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9157,7 +9163,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9169,7 +9175,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9181,7 +9187,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9193,7 +9199,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9205,7 +9211,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9217,7 +9223,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9229,7 +9235,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9241,7 +9247,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9251,7 +9257,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9261,7 +9267,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9271,7 +9277,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9281,7 +9287,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9291,7 +9297,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9301,7 +9307,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9311,7 +9317,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9321,7 +9327,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9331,7 +9337,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9341,7 +9347,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9351,7 +9357,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9361,7 +9367,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9371,7 +9377,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9381,7 +9387,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9391,7 +9397,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9401,7 +9407,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9411,7 +9417,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9421,7 +9427,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9431,7 +9437,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9441,7 +9447,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9451,7 +9457,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9461,7 +9467,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9471,7 +9477,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9481,7 +9487,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9491,7 +9497,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9501,7 +9507,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9511,7 +9517,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9521,7 +9527,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9531,7 +9537,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9541,7 +9547,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9551,7 +9557,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9561,7 +9567,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9571,7 +9577,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9581,7 +9587,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9591,7 +9597,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9601,7 +9607,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lab Print out not show zeros now, added new cut Mg to inventory
</commit_message>
<xml_diff>
--- a/Charge 08 - T06.xlsx
+++ b/Charge 08 - T06.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Elements Data" sheetId="4" r:id="rId1"/>
@@ -1004,7 +1004,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1142,51 +1142,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1453,15 +1414,6 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -1469,7 +1421,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
@@ -1483,26 +1434,16 @@
     <xf numFmtId="0" fontId="12" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1579,6 +1520,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4856,43 +4813,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="173" t="str">
+      <c r="A1" s="163" t="str">
         <f>'Charge 08'!A1:G1</f>
         <v>Charge 08 - T06</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="175"/>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+      <c r="F1" s="164"/>
+      <c r="G1" s="165"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="str">
+      <c r="A2" s="166" t="str">
         <f>"Nominal  " &amp; 'Charge 08'!A3</f>
         <v>Nominal  Mg65Zn30Ca5</v>
       </c>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="178"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="168"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="176" t="str">
+      <c r="A3" s="166" t="str">
         <f>"Actual  " &amp; 'Charge 08'!I3</f>
-        <v>Actual  Mg63.7Zn31.1Ca5.2</v>
-      </c>
-      <c r="B3" s="177"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="177"/>
-      <c r="F3" s="177"/>
-      <c r="G3" s="178"/>
+        <v>Actual  Mg65Zn30Ca5</v>
+      </c>
+      <c r="B3" s="167"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="168"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="171" t="s">
+      <c r="A4" s="161" t="s">
         <v>171</v>
       </c>
       <c r="B4" s="135" t="str">
@@ -4907,36 +4864,36 @@
         <f>'Charge 08'!Q6</f>
         <v>Ca</v>
       </c>
-      <c r="E4" s="163" t="str">
+      <c r="E4" s="155" t="str">
         <f>'Charge 08'!Q7</f>
         <v>D</v>
       </c>
-      <c r="F4" s="159" t="str">
+      <c r="F4" s="153" t="str">
         <f>'Charge 08'!Q8</f>
         <v>E</v>
       </c>
-      <c r="G4" s="154" t="s">
+      <c r="G4" s="150" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="172"/>
-      <c r="B5" s="138" t="s">
+      <c r="A5" s="162"/>
+      <c r="B5" s="184" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="139" t="s">
+      <c r="C5" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="140" t="s">
+      <c r="D5" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="164" t="s">
+      <c r="E5" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="165" t="s">
+      <c r="F5" s="188" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="155" t="s">
+      <c r="G5" s="151" t="s">
         <v>172</v>
       </c>
     </row>
@@ -4945,27 +4902,27 @@
         <v>1</v>
       </c>
       <c r="B6" s="105">
-        <f>'Charge 08'!B14</f>
-        <v>9.6129999999999995</v>
-      </c>
-      <c r="C6" s="141">
-        <f>'Charge 08'!E14</f>
+        <f>IF('Charge 08'!B14=0, "-", 'Charge 08'!B14)</f>
+        <v>4.7270000000000003</v>
+      </c>
+      <c r="C6" s="138">
+        <f>IF('Charge 08'!E14=0,"-",'Charge 08'!E14)</f>
         <v>20.94</v>
       </c>
-      <c r="D6" s="141">
-        <f>'Charge 08'!H14</f>
+      <c r="D6" s="138">
+        <f>IF('Charge 08'!H14=0, "-", 'Charge 08'!H14)</f>
         <v>6.08</v>
       </c>
-      <c r="E6" s="141">
-        <f>'Charge 08'!K14</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="142">
-        <f>'Charge 08'!N14</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="156">
-        <f>COUNTIF(B6:B20, "&lt;&gt;0")</f>
+      <c r="E6" s="138" t="str">
+        <f>IF('Charge 08'!K14=0, "-", 'Charge 08'!K14)</f>
+        <v>-</v>
+      </c>
+      <c r="F6" s="139" t="str">
+        <f>IF('Charge 08'!N14=0, "-", 'Charge 08'!N14)</f>
+        <v>-</v>
+      </c>
+      <c r="G6" s="139">
+        <f>COUNTIF(B6:B20, "&lt;&gt;-")</f>
         <v>6</v>
       </c>
       <c r="H6" s="132" t="str">
@@ -4978,30 +4935,30 @@
         <v>2</v>
       </c>
       <c r="B7" s="108">
-        <f>'Charge 08'!B15</f>
-        <v>8.6839999999999993</v>
+        <f>IF('Charge 08'!B15=0, "-", 'Charge 08'!B15)</f>
+        <v>11.38</v>
       </c>
       <c r="C7" s="107">
-        <f>'Charge 08'!E15</f>
+        <f>IF('Charge 08'!E15=0,"-",'Charge 08'!E15)</f>
         <v>13.51</v>
       </c>
-      <c r="D7" s="107">
-        <f>'Charge 08'!H15</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="107">
-        <f>'Charge 08'!K15</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="106">
-        <f>'Charge 08'!N15</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="157">
-        <f>COUNTIF(C6:C20, "&lt;&gt;0")</f>
+      <c r="D7" s="107" t="str">
+        <f>IF('Charge 08'!H15=0, "-", 'Charge 08'!H15)</f>
+        <v>-</v>
+      </c>
+      <c r="E7" s="107" t="str">
+        <f>IF('Charge 08'!K15=0, "-", 'Charge 08'!K15)</f>
+        <v>-</v>
+      </c>
+      <c r="F7" s="106" t="str">
+        <f>IF('Charge 08'!N15=0, "-", 'Charge 08'!N15)</f>
+        <v>-</v>
+      </c>
+      <c r="G7" s="106">
+        <f>COUNTIF(C6:C20, "&lt;&gt;-")</f>
         <v>4</v>
       </c>
-      <c r="H7" s="158" t="str">
+      <c r="H7" s="152" t="str">
         <f>C4</f>
         <v>Zn</v>
       </c>
@@ -5011,30 +4968,30 @@
         <v>3</v>
       </c>
       <c r="B8" s="108">
-        <f>'Charge 08'!B16</f>
-        <v>7.6580000000000004</v>
+        <f>IF('Charge 08'!B16=0, "-", 'Charge 08'!B16)</f>
+        <v>6.6</v>
       </c>
       <c r="C8" s="107">
-        <f>'Charge 08'!E16</f>
+        <f>IF('Charge 08'!E16=0,"-",'Charge 08'!E16)</f>
         <v>12.664</v>
       </c>
-      <c r="D8" s="107">
-        <f>'Charge 08'!H16</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="107">
-        <f>'Charge 08'!K16</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="106">
-        <f>'Charge 08'!N16</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="157">
-        <f>COUNTIF(D6:D20, "&lt;&gt;0")</f>
+      <c r="D8" s="107" t="str">
+        <f>IF('Charge 08'!H16=0, "-", 'Charge 08'!H16)</f>
+        <v>-</v>
+      </c>
+      <c r="E8" s="107" t="str">
+        <f>IF('Charge 08'!K16=0, "-", 'Charge 08'!K16)</f>
+        <v>-</v>
+      </c>
+      <c r="F8" s="106" t="str">
+        <f>IF('Charge 08'!N16=0, "-", 'Charge 08'!N16)</f>
+        <v>-</v>
+      </c>
+      <c r="G8" s="106">
+        <f>COUNTIF(D6:D20, "&lt;&gt;-")</f>
         <v>1</v>
       </c>
-      <c r="H8" s="153" t="str">
+      <c r="H8" s="149" t="str">
         <f>D4</f>
         <v>Ca</v>
       </c>
@@ -5044,27 +5001,27 @@
         <v>4</v>
       </c>
       <c r="B9" s="108">
-        <f>'Charge 08'!B17</f>
-        <v>7.2839999999999998</v>
+        <f>IF('Charge 08'!B17=0, "-", 'Charge 08'!B17)</f>
+        <v>7.95</v>
       </c>
       <c r="C9" s="107">
-        <f>'Charge 08'!E17</f>
+        <f>IF('Charge 08'!E17=0,"-",'Charge 08'!E17)</f>
         <v>12.114000000000001</v>
       </c>
-      <c r="D9" s="107">
-        <f>'Charge 08'!H17</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="107">
-        <f>'Charge 08'!K17</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="106">
-        <f>'Charge 08'!N17</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="157">
-        <f>COUNTIF(E6:E20, "&lt;&gt;0")</f>
+      <c r="D9" s="107" t="str">
+        <f>IF('Charge 08'!H17=0, "-", 'Charge 08'!H17)</f>
+        <v>-</v>
+      </c>
+      <c r="E9" s="107" t="str">
+        <f>IF('Charge 08'!K17=0, "-", 'Charge 08'!K17)</f>
+        <v>-</v>
+      </c>
+      <c r="F9" s="106" t="str">
+        <f>IF('Charge 08'!N17=0, "-", 'Charge 08'!N17)</f>
+        <v>-</v>
+      </c>
+      <c r="G9" s="106">
+        <f>COUNTIF(E6:E20, "&lt;&gt;-")</f>
         <v>0</v>
       </c>
       <c r="H9" s="137" t="str">
@@ -5077,30 +5034,30 @@
         <v>5</v>
       </c>
       <c r="B10" s="108">
-        <f>'Charge 08'!B18</f>
-        <v>6.3310000000000004</v>
-      </c>
-      <c r="C10" s="107">
-        <f>'Charge 08'!E18</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="107">
-        <f>'Charge 08'!H18</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="107">
-        <f>'Charge 08'!K18</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="106">
-        <f>'Charge 08'!N18</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="160">
-        <f>COUNTIF(F6:F20, "&lt;&gt;0")</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="166" t="str">
+        <f>IF('Charge 08'!B18=0, "-", 'Charge 08'!B18)</f>
+        <v>9.08</v>
+      </c>
+      <c r="C10" s="107" t="str">
+        <f>IF('Charge 08'!E18=0,"-",'Charge 08'!E18)</f>
+        <v>-</v>
+      </c>
+      <c r="D10" s="107" t="str">
+        <f>IF('Charge 08'!H18=0, "-", 'Charge 08'!H18)</f>
+        <v>-</v>
+      </c>
+      <c r="E10" s="107" t="str">
+        <f>IF('Charge 08'!K18=0, "-", 'Charge 08'!K18)</f>
+        <v>-</v>
+      </c>
+      <c r="F10" s="106" t="str">
+        <f>IF('Charge 08'!N18=0, "-", 'Charge 08'!N18)</f>
+        <v>-</v>
+      </c>
+      <c r="G10" s="143">
+        <f>COUNTIF(F6:F20, "&lt;&gt;-")</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="156" t="str">
         <f>F4</f>
         <v>E</v>
       </c>
@@ -5110,30 +5067,30 @@
         <v>6</v>
       </c>
       <c r="B11" s="108">
-        <f>'Charge 08'!B19</f>
-        <v>5.4930000000000003</v>
-      </c>
-      <c r="C11" s="107">
-        <f>'Charge 08'!E19</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="107">
-        <f>'Charge 08'!H19</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="107">
-        <f>'Charge 08'!K19</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="106">
-        <f>'Charge 08'!N19</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="161">
-        <f>COUNTIF(B6:F20, "&lt;&gt;0")</f>
+        <f>IF('Charge 08'!B19=0, "-", 'Charge 08'!B19)</f>
+        <v>7.97</v>
+      </c>
+      <c r="C11" s="107" t="str">
+        <f>IF('Charge 08'!E19=0,"-",'Charge 08'!E19)</f>
+        <v>-</v>
+      </c>
+      <c r="D11" s="107" t="str">
+        <f>IF('Charge 08'!H19=0, "-", 'Charge 08'!H19)</f>
+        <v>-</v>
+      </c>
+      <c r="E11" s="107" t="str">
+        <f>IF('Charge 08'!K19=0, "-", 'Charge 08'!K19)</f>
+        <v>-</v>
+      </c>
+      <c r="F11" s="106" t="str">
+        <f>IF('Charge 08'!N19=0, "-", 'Charge 08'!N19)</f>
+        <v>-</v>
+      </c>
+      <c r="G11" s="183">
+        <f>COUNTIF(B6:F20, "&lt;&gt;-")</f>
         <v>11</v>
       </c>
-      <c r="H11" s="162" t="str">
+      <c r="H11" s="154" t="str">
         <f>G4</f>
         <v>Alloy</v>
       </c>
@@ -5142,25 +5099,25 @@
       <c r="A12" s="27">
         <v>7</v>
       </c>
-      <c r="B12" s="108">
-        <f>'Charge 08'!B20</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="107">
-        <f>'Charge 08'!E20</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="107">
-        <f>'Charge 08'!H20</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="107">
-        <f>'Charge 08'!K20</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="106">
-        <f>'Charge 08'!N20</f>
-        <v>0</v>
+      <c r="B12" s="108" t="str">
+        <f>IF('Charge 08'!B20=0, "-", 'Charge 08'!B20)</f>
+        <v>-</v>
+      </c>
+      <c r="C12" s="107" t="str">
+        <f>IF('Charge 08'!E20=0,"-",'Charge 08'!E20)</f>
+        <v>-</v>
+      </c>
+      <c r="D12" s="107" t="str">
+        <f>IF('Charge 08'!H20=0, "-", 'Charge 08'!H20)</f>
+        <v>-</v>
+      </c>
+      <c r="E12" s="107" t="str">
+        <f>IF('Charge 08'!K20=0, "-", 'Charge 08'!K20)</f>
+        <v>-</v>
+      </c>
+      <c r="F12" s="106" t="str">
+        <f>IF('Charge 08'!N20=0, "-", 'Charge 08'!N20)</f>
+        <v>-</v>
       </c>
       <c r="G12" s="106"/>
     </row>
@@ -5168,25 +5125,25 @@
       <c r="A13" s="27">
         <v>8</v>
       </c>
-      <c r="B13" s="108">
-        <f>'Charge 08'!B21</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="107">
-        <f>'Charge 08'!E21</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="107">
-        <f>'Charge 08'!H21</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="107">
-        <f>'Charge 08'!K21</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="106">
-        <f>'Charge 08'!N21</f>
-        <v>0</v>
+      <c r="B13" s="108" t="str">
+        <f>IF('Charge 08'!B21=0, "-", 'Charge 08'!B21)</f>
+        <v>-</v>
+      </c>
+      <c r="C13" s="107" t="str">
+        <f>IF('Charge 08'!E21=0,"-",'Charge 08'!E21)</f>
+        <v>-</v>
+      </c>
+      <c r="D13" s="107" t="str">
+        <f>IF('Charge 08'!H21=0, "-", 'Charge 08'!H21)</f>
+        <v>-</v>
+      </c>
+      <c r="E13" s="107" t="str">
+        <f>IF('Charge 08'!K21=0, "-", 'Charge 08'!K21)</f>
+        <v>-</v>
+      </c>
+      <c r="F13" s="106" t="str">
+        <f>IF('Charge 08'!N21=0, "-", 'Charge 08'!N21)</f>
+        <v>-</v>
       </c>
       <c r="G13" s="106"/>
     </row>
@@ -5194,25 +5151,25 @@
       <c r="A14" s="27">
         <v>9</v>
       </c>
-      <c r="B14" s="108">
-        <f>'Charge 08'!B22</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="107">
-        <f>'Charge 08'!E22</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="107">
-        <f>'Charge 08'!H22</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="107">
-        <f>'Charge 08'!K22</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="106">
-        <f>'Charge 08'!N22</f>
-        <v>0</v>
+      <c r="B14" s="108" t="str">
+        <f>IF('Charge 08'!B22=0, "-", 'Charge 08'!B22)</f>
+        <v>-</v>
+      </c>
+      <c r="C14" s="107" t="str">
+        <f>IF('Charge 08'!E22=0,"-",'Charge 08'!E22)</f>
+        <v>-</v>
+      </c>
+      <c r="D14" s="107" t="str">
+        <f>IF('Charge 08'!H22=0, "-", 'Charge 08'!H22)</f>
+        <v>-</v>
+      </c>
+      <c r="E14" s="107" t="str">
+        <f>IF('Charge 08'!K22=0, "-", 'Charge 08'!K22)</f>
+        <v>-</v>
+      </c>
+      <c r="F14" s="106" t="str">
+        <f>IF('Charge 08'!N22=0, "-", 'Charge 08'!N22)</f>
+        <v>-</v>
       </c>
       <c r="G14" s="106"/>
     </row>
@@ -5220,25 +5177,25 @@
       <c r="A15" s="27">
         <v>10</v>
       </c>
-      <c r="B15" s="108">
-        <f>'Charge 08'!B23</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="107">
-        <f>'Charge 08'!E23</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="107">
-        <f>'Charge 08'!H23</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="107">
-        <f>'Charge 08'!K23</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="106">
-        <f>'Charge 08'!N23</f>
-        <v>0</v>
+      <c r="B15" s="108" t="str">
+        <f>IF('Charge 08'!B23=0, "-", 'Charge 08'!B23)</f>
+        <v>-</v>
+      </c>
+      <c r="C15" s="107" t="str">
+        <f>IF('Charge 08'!E23=0,"-",'Charge 08'!E23)</f>
+        <v>-</v>
+      </c>
+      <c r="D15" s="107" t="str">
+        <f>IF('Charge 08'!H23=0, "-", 'Charge 08'!H23)</f>
+        <v>-</v>
+      </c>
+      <c r="E15" s="107" t="str">
+        <f>IF('Charge 08'!K23=0, "-", 'Charge 08'!K23)</f>
+        <v>-</v>
+      </c>
+      <c r="F15" s="106" t="str">
+        <f>IF('Charge 08'!N23=0, "-", 'Charge 08'!N23)</f>
+        <v>-</v>
       </c>
       <c r="G15" s="106"/>
     </row>
@@ -5246,25 +5203,25 @@
       <c r="A16" s="27">
         <v>11</v>
       </c>
-      <c r="B16" s="108">
-        <f>'Charge 08'!B24</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="107">
-        <f>'Charge 08'!E24</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="107">
-        <f>'Charge 08'!H24</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="107">
-        <f>'Charge 08'!K24</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="106">
-        <f>'Charge 08'!N24</f>
-        <v>0</v>
+      <c r="B16" s="108" t="str">
+        <f>IF('Charge 08'!B24=0, "-", 'Charge 08'!B24)</f>
+        <v>-</v>
+      </c>
+      <c r="C16" s="107" t="str">
+        <f>IF('Charge 08'!E24=0,"-",'Charge 08'!E24)</f>
+        <v>-</v>
+      </c>
+      <c r="D16" s="107" t="str">
+        <f>IF('Charge 08'!H24=0, "-", 'Charge 08'!H24)</f>
+        <v>-</v>
+      </c>
+      <c r="E16" s="107" t="str">
+        <f>IF('Charge 08'!K24=0, "-", 'Charge 08'!K24)</f>
+        <v>-</v>
+      </c>
+      <c r="F16" s="106" t="str">
+        <f>IF('Charge 08'!N24=0, "-", 'Charge 08'!N24)</f>
+        <v>-</v>
       </c>
       <c r="G16" s="106"/>
     </row>
@@ -5272,25 +5229,25 @@
       <c r="A17" s="27">
         <v>12</v>
       </c>
-      <c r="B17" s="108">
-        <f>'Charge 08'!B25</f>
-        <v>0</v>
-      </c>
-      <c r="C17" s="107">
-        <f>'Charge 08'!E25</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="107">
-        <f>'Charge 08'!H25</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="107">
-        <f>'Charge 08'!K25</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="106">
-        <f>'Charge 08'!N25</f>
-        <v>0</v>
+      <c r="B17" s="108" t="str">
+        <f>IF('Charge 08'!B25=0, "-", 'Charge 08'!B25)</f>
+        <v>-</v>
+      </c>
+      <c r="C17" s="107" t="str">
+        <f>IF('Charge 08'!E25=0,"-",'Charge 08'!E25)</f>
+        <v>-</v>
+      </c>
+      <c r="D17" s="107" t="str">
+        <f>IF('Charge 08'!H25=0, "-", 'Charge 08'!H25)</f>
+        <v>-</v>
+      </c>
+      <c r="E17" s="107" t="str">
+        <f>IF('Charge 08'!K25=0, "-", 'Charge 08'!K25)</f>
+        <v>-</v>
+      </c>
+      <c r="F17" s="106" t="str">
+        <f>IF('Charge 08'!N25=0, "-", 'Charge 08'!N25)</f>
+        <v>-</v>
       </c>
       <c r="G17" s="106"/>
     </row>
@@ -5298,25 +5255,25 @@
       <c r="A18" s="27">
         <v>13</v>
       </c>
-      <c r="B18" s="108">
-        <f>'Charge 08'!B26</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="107">
-        <f>'Charge 08'!E26</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="107">
-        <f>'Charge 08'!H26</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="107">
-        <f>'Charge 08'!K26</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="106">
-        <f>'Charge 08'!N26</f>
-        <v>0</v>
+      <c r="B18" s="108" t="str">
+        <f>IF('Charge 08'!B26=0, "-", 'Charge 08'!B26)</f>
+        <v>-</v>
+      </c>
+      <c r="C18" s="107" t="str">
+        <f>IF('Charge 08'!E26=0,"-",'Charge 08'!E26)</f>
+        <v>-</v>
+      </c>
+      <c r="D18" s="107" t="str">
+        <f>IF('Charge 08'!H26=0, "-", 'Charge 08'!H26)</f>
+        <v>-</v>
+      </c>
+      <c r="E18" s="107" t="str">
+        <f>IF('Charge 08'!K26=0, "-", 'Charge 08'!K26)</f>
+        <v>-</v>
+      </c>
+      <c r="F18" s="106" t="str">
+        <f>IF('Charge 08'!N26=0, "-", 'Charge 08'!N26)</f>
+        <v>-</v>
       </c>
       <c r="G18" s="106"/>
     </row>
@@ -5324,25 +5281,25 @@
       <c r="A19" s="27">
         <v>14</v>
       </c>
-      <c r="B19" s="108">
-        <f>'Charge 08'!B27</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="107">
-        <f>'Charge 08'!E27</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="107">
-        <f>'Charge 08'!H27</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="107">
-        <f>'Charge 08'!K27</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="106">
-        <f>'Charge 08'!N27</f>
-        <v>0</v>
+      <c r="B19" s="108" t="str">
+        <f>IF('Charge 08'!B27=0, "-", 'Charge 08'!B27)</f>
+        <v>-</v>
+      </c>
+      <c r="C19" s="107" t="str">
+        <f>IF('Charge 08'!E27=0,"-",'Charge 08'!E27)</f>
+        <v>-</v>
+      </c>
+      <c r="D19" s="107" t="str">
+        <f>IF('Charge 08'!H27=0, "-", 'Charge 08'!H27)</f>
+        <v>-</v>
+      </c>
+      <c r="E19" s="107" t="str">
+        <f>IF('Charge 08'!K27=0, "-", 'Charge 08'!K27)</f>
+        <v>-</v>
+      </c>
+      <c r="F19" s="106" t="str">
+        <f>IF('Charge 08'!N27=0, "-", 'Charge 08'!N27)</f>
+        <v>-</v>
       </c>
       <c r="G19" s="106"/>
     </row>
@@ -5350,62 +5307,62 @@
       <c r="A20" s="27">
         <v>15</v>
       </c>
-      <c r="B20" s="145">
-        <f>'Charge 08'!B28</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="114">
-        <f>'Charge 08'!E28</f>
-        <v>0</v>
-      </c>
-      <c r="D20" s="114">
-        <f>'Charge 08'!H28</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="114">
-        <f>'Charge 08'!K28</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="146">
-        <f>'Charge 08'!N28</f>
-        <v>0</v>
+      <c r="B20" s="142" t="str">
+        <f>IF('Charge 08'!B28=0, "-", 'Charge 08'!B28)</f>
+        <v>-</v>
+      </c>
+      <c r="C20" s="114" t="str">
+        <f>IF('Charge 08'!E28=0,"-",'Charge 08'!E28)</f>
+        <v>-</v>
+      </c>
+      <c r="D20" s="114" t="str">
+        <f>IF('Charge 08'!H28=0, "-", 'Charge 08'!H28)</f>
+        <v>-</v>
+      </c>
+      <c r="E20" s="114" t="str">
+        <f>IF('Charge 08'!K28=0, "-", 'Charge 08'!K28)</f>
+        <v>-</v>
+      </c>
+      <c r="F20" s="143" t="str">
+        <f>IF('Charge 08'!N28=0, "-", 'Charge 08'!N28)</f>
+        <v>-</v>
       </c>
       <c r="G20" s="106"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="147" t="s">
+      <c r="A21" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="72">
+      <c r="B21" s="77">
         <f>SUM(B6:B20)</f>
-        <v>45.063000000000002</v>
-      </c>
-      <c r="C21" s="36">
+        <v>47.707000000000001</v>
+      </c>
+      <c r="C21" s="37">
         <f>SUM(C6:C20)</f>
         <v>59.228000000000009</v>
       </c>
-      <c r="D21" s="148">
+      <c r="D21" s="69">
         <f>SUM(D6:D20)</f>
         <v>6.08</v>
       </c>
-      <c r="E21" s="36">
+      <c r="E21" s="69">
         <f>SUM(E6:E20)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="149">
+      <c r="F21" s="110">
         <f>SUM(F6:F20)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="149">
+      <c r="G21" s="145">
         <f>SUM(B21:F21)</f>
-        <v>110.37100000000001</v>
+        <v>113.015</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="B22" s="150">
+      <c r="B22" s="146">
         <f>'Charge 08'!F4</f>
         <v>47.710999999999999</v>
       </c>
@@ -5421,7 +5378,7 @@
         <f>'Charge 08'!F7</f>
         <v>0</v>
       </c>
-      <c r="F22" s="143">
+      <c r="F22" s="140">
         <f>'Charge 08'!F8</f>
         <v>0</v>
       </c>
@@ -5431,22 +5388,22 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="152" t="s">
+      <c r="A23" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="151">
+      <c r="B23" s="147">
         <f>B21-B22</f>
-        <v>-2.6479999999999961</v>
-      </c>
-      <c r="C23" s="144">
+        <v>-3.9999999999977831E-3</v>
+      </c>
+      <c r="C23" s="141">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
         <v>-8.9999999999932356E-3</v>
       </c>
-      <c r="D23" s="144">
+      <c r="D23" s="141">
         <f t="shared" si="0"/>
         <v>2.8000000000000469E-2</v>
       </c>
-      <c r="E23" s="144">
+      <c r="E23" s="141">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5456,7 +5413,7 @@
       </c>
       <c r="G23" s="113">
         <f t="shared" si="0"/>
-        <v>-2.6289999999999907</v>
+        <v>1.5000000000000568E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -5480,7 +5437,7 @@
   </sheetPr>
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
@@ -5504,15 +5461,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="169" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
-      <c r="F1" s="179"/>
-      <c r="G1" s="179"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
     </row>
     <row r="2" spans="1:28" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="54" t="s">
@@ -5552,7 +5509,7 @@
       </c>
       <c r="I3" s="62" t="str">
         <f>Q4 &amp; ROUND(N4,3)*100 &amp; IF(N5=0, "", Q5 &amp; ROUND(N5,3)*100) &amp; IF(N6=0, "", Q6 &amp; ROUND(N6,3)*100) &amp; IF(N7=0, "", Q7 &amp; ROUND(N7,3)*100) &amp; IF(N8=0, "", Q8 &amp; ROUND(N8,3)*100)</f>
-        <v>Mg63.7Zn31.1Ca5.2</v>
+        <v>Mg65Zn30Ca5</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="s">
@@ -5658,19 +5615,19 @@
       <c r="J4" s="26"/>
       <c r="K4" s="72">
         <f>B29</f>
-        <v>45.063000000000002</v>
+        <v>47.707000000000001</v>
       </c>
       <c r="L4" s="73">
         <f>K4/$K$9</f>
-        <v>0.40828659702276865</v>
+        <v>0.42212980577799408</v>
       </c>
       <c r="M4" s="23">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>1.6798461099476185E-2</v>
+        <v>1.7368023278255259E-2</v>
       </c>
       <c r="N4" s="115">
         <f>M4/$M$9</f>
-        <v>0.63677542870187764</v>
+        <v>0.64985738278710559</v>
       </c>
       <c r="P4" s="15">
         <v>1</v>
@@ -5759,15 +5716,15 @@
       </c>
       <c r="L5" s="76">
         <f>K5/$K$9</f>
-        <v>0.53662646890940557</v>
+        <v>0.5240720258372783</v>
       </c>
       <c r="M5" s="24">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>8.2075566502922137E-3</v>
+        <v>8.0155398402813969E-3</v>
       </c>
       <c r="N5" s="116">
         <f>M5/$M$9</f>
-        <v>0.31112197561642962</v>
+        <v>0.29991655692635161</v>
       </c>
       <c r="P5" s="15">
         <v>2</v>
@@ -5856,15 +5813,15 @@
       </c>
       <c r="L6" s="76">
         <f>K6/$K$9</f>
-        <v>5.5086934067825784E-2</v>
+        <v>5.3798168384727695E-2</v>
       </c>
       <c r="M6" s="24">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>1.3744930901698133E-3</v>
+        <v>1.3423366531445603E-3</v>
       </c>
       <c r="N6" s="116">
         <f>M6/$M$9</f>
-        <v>5.2102595681692745E-2</v>
+        <v>5.0226060286542765E-2</v>
       </c>
       <c r="P6" s="15">
         <v>3</v>
@@ -6127,10 +6084,10 @@
         <f>SUM(E4:E8)</f>
         <v>1</v>
       </c>
-      <c r="F9" s="168">
+      <c r="F9" s="158">
         <v>113</v>
       </c>
-      <c r="G9" s="149">
+      <c r="G9" s="145">
         <f>SUM(G4:G8)</f>
         <v>39.652683313052009</v>
       </c>
@@ -6140,7 +6097,7 @@
       </c>
       <c r="K9" s="117">
         <f>SUM(K4:K8)</f>
-        <v>110.37100000000001</v>
+        <v>113.015</v>
       </c>
       <c r="L9" s="83">
         <f>SUM(L4:L8)</f>
@@ -6148,7 +6105,7 @@
       </c>
       <c r="M9" s="118">
         <f>SUM(M4:M8)</f>
-        <v>2.6380510839938212E-2</v>
+        <v>2.6725899771681216E-2</v>
       </c>
       <c r="N9" s="84">
         <f>SUM(N4:N8)</f>
@@ -6161,7 +6118,7 @@
         <f>Q4 &amp; R4*100 &amp; Q5 &amp; R5*100 &amp; Q6 &amp; R6*100 &amp; Q7 &amp; R7*100 &amp; Q8 &amp; R8*100</f>
         <v>Mg65Zn30Ca5D0E0</v>
       </c>
-      <c r="R9" s="167">
+      <c r="R9" s="157">
         <f>SUM(R4:R8)</f>
         <v>1</v>
       </c>
@@ -6181,18 +6138,18 @@
         <v>812.5</v>
       </c>
       <c r="Y9" s="114"/>
-      <c r="Z9" s="170">
+      <c r="Z9" s="160">
         <f>(MAX(Z4:Z8)-SMALL(Z4:Z8,COUNTIF(Z4:Z8,"&lt;=0")+1))/MAX(Z4:Z8)</f>
         <v>0.16874999999999998</v>
       </c>
-      <c r="AA9" s="170">
+      <c r="AA9" s="160">
         <f>(MAX(AA4:AA8)-SMALL(AA4:AA8,COUNTIF(AA4:AA8,"&lt;=0")+1))/MAX(AA4:AA8)</f>
         <v>0.2421052631578948</v>
       </c>
-      <c r="AB9" s="146"/>
+      <c r="AB9" s="143"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="F10" s="169">
+      <c r="F10" s="159">
         <f>G10*U9</f>
         <v>0</v>
       </c>
@@ -6209,35 +6166,35 @@
       </c>
     </row>
     <row r="12" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="183" t="str">
+      <c r="A12" s="173" t="str">
         <f>$Q$4</f>
         <v>Mg</v>
       </c>
-      <c r="B12" s="184"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="87"/>
-      <c r="D12" s="185" t="str">
+      <c r="D12" s="175" t="str">
         <f>$Q$5</f>
         <v>Zn</v>
       </c>
-      <c r="E12" s="186"/>
+      <c r="E12" s="176"/>
       <c r="F12" s="87"/>
-      <c r="G12" s="187" t="str">
+      <c r="G12" s="177" t="str">
         <f>$Q$6</f>
         <v>Ca</v>
       </c>
-      <c r="H12" s="188"/>
+      <c r="H12" s="178"/>
       <c r="I12" s="88"/>
-      <c r="J12" s="189" t="str">
+      <c r="J12" s="179" t="str">
         <f>$Q$7</f>
         <v>D</v>
       </c>
-      <c r="K12" s="190"/>
+      <c r="K12" s="180"/>
       <c r="L12" s="87"/>
-      <c r="M12" s="191" t="str">
+      <c r="M12" s="181" t="str">
         <f>$Q$8</f>
         <v>E</v>
       </c>
-      <c r="N12" s="192"/>
+      <c r="N12" s="182"/>
       <c r="P12" s="89" t="s">
         <v>90</v>
       </c>
@@ -6303,7 +6260,7 @@
       </c>
       <c r="B14" s="106">
         <f>A!C2</f>
-        <v>9.6129999999999995</v>
+        <v>4.7270000000000003</v>
       </c>
       <c r="C14" s="107"/>
       <c r="D14" s="127">
@@ -6356,7 +6313,7 @@
       </c>
       <c r="B15" s="106">
         <f>A!C3</f>
-        <v>8.6839999999999993</v>
+        <v>11.38</v>
       </c>
       <c r="C15" s="107"/>
       <c r="D15" s="127">
@@ -6409,7 +6366,7 @@
       </c>
       <c r="B16" s="106">
         <f>A!C4</f>
-        <v>7.6580000000000004</v>
+        <v>6.6</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="127">
@@ -6462,7 +6419,7 @@
       </c>
       <c r="B17" s="106">
         <f>A!C5</f>
-        <v>7.2839999999999998</v>
+        <v>7.95</v>
       </c>
       <c r="C17" s="107"/>
       <c r="D17" s="127">
@@ -6515,7 +6472,7 @@
       </c>
       <c r="B18" s="106">
         <f>A!C6</f>
-        <v>6.3310000000000004</v>
+        <v>9.08</v>
       </c>
       <c r="C18" s="107"/>
       <c r="D18" s="127">
@@ -6570,7 +6527,7 @@
       </c>
       <c r="B19" s="106">
         <f>A!C7</f>
-        <v>5.4930000000000003</v>
+        <v>7.97</v>
       </c>
       <c r="C19" s="107"/>
       <c r="D19" s="127">
@@ -7017,7 +6974,7 @@
       </c>
       <c r="B29" s="110">
         <f>SUM(B14:B28)</f>
-        <v>45.063000000000002</v>
+        <v>47.707000000000001</v>
       </c>
       <c r="C29" s="107"/>
       <c r="D29" s="109" t="s">
@@ -7058,7 +7015,7 @@
       </c>
       <c r="B30" s="113">
         <f>B29-$F$4</f>
-        <v>-2.6479999999999961</v>
+        <v>-3.9999999999977831E-3</v>
       </c>
       <c r="C30" s="114"/>
       <c r="D30" s="112" t="s">
@@ -7095,36 +7052,36 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="180" t="s">
+      <c r="A32" s="170" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="181"/>
-      <c r="C32" s="181"/>
-      <c r="D32" s="181"/>
-      <c r="E32" s="181"/>
-      <c r="F32" s="181"/>
-      <c r="G32" s="181"/>
-      <c r="H32" s="181"/>
-      <c r="I32" s="181"/>
-      <c r="J32" s="181"/>
-      <c r="K32" s="181"/>
-      <c r="L32" s="181"/>
-      <c r="M32" s="181"/>
-      <c r="N32" s="181"/>
-      <c r="O32" s="181"/>
-      <c r="P32" s="181"/>
-      <c r="Q32" s="181"/>
-      <c r="R32" s="181"/>
-      <c r="S32" s="181"/>
-      <c r="T32" s="181"/>
-      <c r="U32" s="181"/>
-      <c r="V32" s="181"/>
-      <c r="W32" s="181"/>
-      <c r="X32" s="181"/>
-      <c r="Y32" s="181"/>
-      <c r="Z32" s="181"/>
-      <c r="AA32" s="181"/>
-      <c r="AB32" s="182"/>
+      <c r="B32" s="171"/>
+      <c r="C32" s="171"/>
+      <c r="D32" s="171"/>
+      <c r="E32" s="171"/>
+      <c r="F32" s="171"/>
+      <c r="G32" s="171"/>
+      <c r="H32" s="171"/>
+      <c r="I32" s="171"/>
+      <c r="J32" s="171"/>
+      <c r="K32" s="171"/>
+      <c r="L32" s="171"/>
+      <c r="M32" s="171"/>
+      <c r="N32" s="171"/>
+      <c r="O32" s="171"/>
+      <c r="P32" s="171"/>
+      <c r="Q32" s="171"/>
+      <c r="R32" s="171"/>
+      <c r="S32" s="171"/>
+      <c r="T32" s="171"/>
+      <c r="U32" s="171"/>
+      <c r="V32" s="171"/>
+      <c r="W32" s="171"/>
+      <c r="X32" s="171"/>
+      <c r="Y32" s="171"/>
+      <c r="Z32" s="171"/>
+      <c r="AA32" s="171"/>
+      <c r="AB32" s="172"/>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="42"/>
@@ -8428,7 +8385,7 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -8464,19 +8421,19 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="126">
-        <v>9.6129999999999995</v>
+      <c r="A2" s="125">
+        <v>4.7270000000000003</v>
       </c>
       <c r="B2" s="125">
         <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>9.6129999999999995</v>
+        <f>IF(A2=0, 0, A2*B2)</f>
+        <v>4.7270000000000003</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>45.063000000000002</v>
+        <v>47.707000000000001</v>
       </c>
       <c r="E2" s="128" t="s">
         <v>109</v>
@@ -8488,14 +8445,14 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="125">
-        <v>8.6839999999999993</v>
+        <v>11.38</v>
       </c>
       <c r="B3" s="125">
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>8.6839999999999993</v>
+        <f>IF(A3=0, 0, A3*B3)</f>
+        <v>11.38</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="128" t="s">
@@ -8503,19 +8460,19 @@
       </c>
       <c r="F3" s="130">
         <f>SUM(C:C)</f>
-        <v>45.063000000000002</v>
+        <v>47.707000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="125">
-        <v>7.6580000000000004</v>
+        <v>6.6</v>
       </c>
       <c r="B4" s="125">
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>7.6580000000000004</v>
+        <f>IF(A4=0, 0, A4*B4)</f>
+        <v>6.6</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="128" t="s">
@@ -8523,156 +8480,174 @@
       </c>
       <c r="F4" s="130">
         <f>F3-F2</f>
-        <v>-2.6479999999999961</v>
+        <v>-3.9999999999977831E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="125">
-        <v>7.2839999999999998</v>
+      <c r="A5" s="126">
+        <v>7.95</v>
       </c>
       <c r="B5" s="125">
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>7.2839999999999998</v>
+        <f>IF(A5=0, 0, A5*B5)</f>
+        <v>7.95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="126">
-        <v>6.3310000000000004</v>
+        <v>9.08</v>
       </c>
       <c r="B6" s="125">
         <v>1</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>6.3310000000000004</v>
+        <f>IF(A6=0, 0, A6*B6)</f>
+        <v>9.08</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="126">
-        <v>5.4930000000000003</v>
+      <c r="A7" s="125">
+        <v>7.97</v>
       </c>
       <c r="B7" s="125">
         <v>1</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>5.4930000000000003</v>
+        <f>IF(A7=0, 0, A7*B7)</f>
+        <v>7.97</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="126">
-        <v>4.8339999999999996</v>
+        <v>9.6129999999999995</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="125">
-        <v>4.7270000000000003</v>
+        <v>8.6839999999999993</v>
       </c>
       <c r="B9" s="125">
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="126"/>
+      <c r="A10" s="125">
+        <v>7.6580000000000004</v>
+      </c>
       <c r="B10" s="125">
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="126"/>
+      <c r="A11" s="125">
+        <v>7.2839999999999998</v>
+      </c>
       <c r="B11" s="125">
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="125"/>
+      <c r="A12" s="126">
+        <v>6.3310000000000004</v>
+      </c>
       <c r="B12" s="125">
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
+      <c r="A13" s="126">
+        <v>5.4930000000000003</v>
+      </c>
       <c r="B13" s="125">
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="126"/>
+      <c r="A14" s="126">
+        <v>4.8339999999999996</v>
+      </c>
       <c r="B14" s="125">
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="126"/>
+      <c r="A15" s="126">
+        <v>15.55</v>
+      </c>
       <c r="B15" s="125">
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="126"/>
+      <c r="A16" s="126">
+        <v>13.8</v>
+      </c>
       <c r="B16" s="125">
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="125"/>
+      <c r="A17" s="126">
+        <v>7.91</v>
+      </c>
       <c r="B17" s="125">
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="126"/>
+      <c r="A18" s="126">
+        <v>8.1300000000000008</v>
+      </c>
       <c r="B18" s="125">
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
@@ -8682,7 +8657,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
@@ -8692,7 +8667,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
@@ -8702,7 +8677,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
@@ -8712,7 +8687,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
@@ -8722,7 +8697,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
@@ -8732,7 +8707,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
@@ -8742,7 +8717,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
@@ -8752,7 +8727,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
@@ -8762,7 +8737,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -8772,7 +8747,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -8782,7 +8757,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -8792,7 +8767,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -8802,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -8812,7 +8787,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -8822,7 +8797,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -8832,7 +8807,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8842,7 +8817,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -8852,7 +8827,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -8862,7 +8837,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -8872,7 +8847,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -8882,7 +8857,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -8892,7 +8867,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -8902,7 +8877,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -8912,7 +8887,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -8922,7 +8897,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -8932,7 +8907,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -8942,7 +8917,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -8952,7 +8927,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -8962,7 +8937,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -8972,7 +8947,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -8982,7 +8957,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -8992,7 +8967,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -9002,14 +8977,14 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition descending="1" ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>